<commit_message>
changes made. my trying shit out file is becoming a mess.
</commit_message>
<xml_diff>
--- a/regressor and classifier importances.xlsx
+++ b/regressor and classifier importances.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minna\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a38cc7a04266740c/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="389" documentId="8_{E93A6E45-9447-44B2-A386-D641E629DBB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0C4DF848-B10D-4A38-A3B4-226DB8C321D8}"/>
+  <xr:revisionPtr revIDLastSave="435" documentId="8_{E93A6E45-9447-44B2-A386-D641E629DBB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EE6DDEE8-17E3-438D-B0AD-9C9C87EFEE5C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{789FB943-771A-4B19-9A66-979F3CA78A6C}"/>
+    <workbookView xWindow="3552" yWindow="1200" windowWidth="13668" windowHeight="4500" firstSheet="1" activeTab="1" xr2:uid="{789FB943-771A-4B19-9A66-979F3CA78A6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Original Importances" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="Heatmaps" sheetId="3" r:id="rId3"/>
     <sheet name="chi - 2" sheetId="4" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="147">
   <si>
     <t>Classifier Importances</t>
   </si>
@@ -485,8 +488,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000%"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -567,34 +570,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1903,396 +1906,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Trade-In</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="percentStacked"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Distribution Data Tables (mess)'!$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Loyal</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Distribution Data Tables (mess)'!$G$2:$G$3</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Trade-In</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>No Trade-In</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Distribution Data Tables (mess)'!$I$2:$I$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>61077</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>62477</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FF9D-49F0-82BE-0652835F1EBF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Distribution Data Tables (mess)'!$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Nonloyal</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Distribution Data Tables (mess)'!$G$2:$G$3</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Trade-In</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>No Trade-In</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Distribution Data Tables (mess)'!$H$2:$H$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>106782</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>131220</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-FF9D-49F0-82BE-0652835F1EBF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
-        <c:axId val="2010917280"/>
-        <c:axId val="2015821296"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2010917280"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2015821296"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2015821296"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2010917280"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2414,46 +2027,6 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4513,511 +4086,6 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -5169,45 +4237,20 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78A77B9E-82EA-48F6-AA0D-83D0E2D0ECEC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5832,10 +4875,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58B855E-757F-44CC-B7FE-FF60EBDD6187}">
-  <dimension ref="B1:Z474"/>
+  <dimension ref="B1:AC474"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30:J48"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5843,7 +4886,7 @@
     <col min="15" max="15" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:29" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>18</v>
       </c>
@@ -5857,7 +4900,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>15</v>
       </c>
@@ -5872,16 +4915,16 @@
         <v>0.38706849171661128</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2">
-        <v>106782</v>
+        <v>131220</v>
       </c>
       <c r="I2">
-        <v>61077</v>
+        <v>62477</v>
       </c>
       <c r="J2" s="3">
-        <f>I2/SUM(H2:I2)</f>
+        <f>I3/SUM(H3:I3)</f>
         <v>0.36385895304988114</v>
       </c>
       <c r="P2" t="s">
@@ -5893,8 +4936,17 @@
       <c r="R2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+      <c r="U2" t="s">
+        <v>92</v>
+      </c>
+      <c r="V2" t="s">
+        <v>93</v>
+      </c>
+      <c r="W2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -5909,16 +4961,16 @@
         <v>0.32957725732803062</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3">
-        <v>131220</v>
+        <v>106782</v>
       </c>
       <c r="I3">
-        <v>62477</v>
+        <v>61077</v>
       </c>
       <c r="J3" s="3">
-        <f>I3/SUM(H3:I3)</f>
+        <f>I2/SUM(H2:I2)</f>
         <v>0.32255016856223895</v>
       </c>
       <c r="M3" t="s">
@@ -5944,12 +4996,22 @@
       <c r="T3" t="s">
         <v>87</v>
       </c>
-      <c r="W3" s="6">
+      <c r="U3">
+        <v>2</v>
+      </c>
+      <c r="W3">
+        <v>5000</v>
+      </c>
+      <c r="Y3">
+        <f>SUM(V3:V47)/SUM(U3:V47)</f>
+        <v>0.76755468032614593</v>
+      </c>
+      <c r="Z3" s="6">
         <f>SUM(R3:R47)/(SUM(Q3:Q47)+SUM(R3:R47))</f>
         <v>0.34172852891391653</v>
       </c>
     </row>
-    <row r="4" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O4" t="str">
         <f t="shared" ref="O4:O47" si="0">T4&amp;" ("&amp;S4&amp;")"</f>
         <v>BENTLEY/MASERATI (0.00%)</v>
@@ -5970,14 +5032,20 @@
       <c r="T4" t="s">
         <v>88</v>
       </c>
-      <c r="X4" t="s">
+      <c r="U4">
+        <v>4</v>
+      </c>
+      <c r="W4">
+        <v>57500</v>
+      </c>
+      <c r="AA4" t="s">
         <v>18</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AB4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O5" t="str">
         <f t="shared" si="0"/>
         <v>LOTUS (0.00%)</v>
@@ -5998,21 +5066,27 @@
       <c r="T5" t="s">
         <v>59</v>
       </c>
-      <c r="W5" t="s">
+      <c r="U5">
+        <v>4</v>
+      </c>
+      <c r="W5">
+        <v>23750</v>
+      </c>
+      <c r="Z5" t="s">
         <v>90</v>
       </c>
-      <c r="X5">
+      <c r="AA5">
         <v>146486</v>
       </c>
-      <c r="Y5">
+      <c r="AB5">
         <v>78098</v>
       </c>
-      <c r="Z5" s="3">
-        <f>Y5/SUM(X5:Y5)</f>
+      <c r="AC5" s="3">
+        <f>AB5/SUM(AA5:AB5)</f>
         <v>0.34774516439283298</v>
       </c>
     </row>
-    <row r="6" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O6" t="str">
         <f t="shared" si="0"/>
         <v>PLYMOUTH (0.00%)</v>
@@ -6033,21 +5107,27 @@
       <c r="T6" t="s">
         <v>68</v>
       </c>
-      <c r="W6" t="s">
+      <c r="U6">
+        <v>8</v>
+      </c>
+      <c r="W6">
+        <v>5000</v>
+      </c>
+      <c r="Z6" t="s">
         <v>91</v>
       </c>
-      <c r="X6">
+      <c r="AA6">
         <v>91516</v>
       </c>
-      <c r="Y6">
+      <c r="AB6">
         <v>45456</v>
       </c>
-      <c r="Z6" s="3">
-        <f>Y6/SUM(X6:Y6)</f>
+      <c r="AC6" s="3">
+        <f>AB6/SUM(AA6:AB6)</f>
         <v>0.33186344654381916</v>
       </c>
     </row>
-    <row r="7" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O7" t="str">
         <f t="shared" si="0"/>
         <v>GEO (0.00%)</v>
@@ -6068,9 +5148,15 @@
       <c r="T7" t="s">
         <v>46</v>
       </c>
-      <c r="Z7" s="3"/>
-    </row>
-    <row r="8" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+      <c r="U7">
+        <v>12</v>
+      </c>
+      <c r="W7">
+        <v>5000</v>
+      </c>
+      <c r="AC7" s="3"/>
+    </row>
+    <row r="8" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O8" t="str">
         <f t="shared" si="0"/>
         <v>SAAB (0.01%)</v>
@@ -6091,15 +5177,21 @@
       <c r="T8" t="s">
         <v>71</v>
       </c>
-      <c r="X8" t="s">
+      <c r="U8">
+        <v>25</v>
+      </c>
+      <c r="W8">
+        <v>7400</v>
+      </c>
+      <c r="AA8" t="s">
         <v>18</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="AB8" t="s">
         <v>17</v>
       </c>
-      <c r="Z8" s="3"/>
-    </row>
-    <row r="9" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC8" s="3"/>
+    </row>
+    <row r="9" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O9" t="str">
         <f t="shared" si="0"/>
         <v>OLDSMOBILE (0.01%)</v>
@@ -6120,21 +5212,30 @@
       <c r="T9" t="s">
         <v>67</v>
       </c>
-      <c r="W9" t="s">
+      <c r="U9">
+        <v>39</v>
+      </c>
+      <c r="V9">
+        <v>8</v>
+      </c>
+      <c r="W9">
+        <v>6276.5957446808497</v>
+      </c>
+      <c r="Z9" t="s">
         <v>92</v>
       </c>
-      <c r="X9">
+      <c r="AA9">
         <v>52909</v>
       </c>
-      <c r="Y9">
+      <c r="AB9">
         <v>31133</v>
       </c>
-      <c r="Z9" s="3">
-        <f>Y9/SUM(X9:Y9)</f>
+      <c r="AC9" s="3">
+        <f>AB9/SUM(AA9:AB9)</f>
         <v>0.37044572951619431</v>
       </c>
     </row>
-    <row r="10" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O10" t="str">
         <f t="shared" si="0"/>
         <v>ISUZU (0.02%)</v>
@@ -6155,21 +5256,30 @@
       <c r="T10" t="s">
         <v>52</v>
       </c>
-      <c r="W10" t="s">
+      <c r="U10">
+        <v>30</v>
+      </c>
+      <c r="V10">
+        <v>36</v>
+      </c>
+      <c r="W10">
+        <v>10984.848484848451</v>
+      </c>
+      <c r="Z10" t="s">
         <v>93</v>
       </c>
-      <c r="X10">
+      <c r="AA10">
         <v>185093</v>
       </c>
-      <c r="Y10">
+      <c r="AB10">
         <v>92421</v>
       </c>
-      <c r="Z10" s="3">
-        <f>Y10/SUM(X10:Y10)</f>
+      <c r="AC10" s="3">
+        <f>AB10/SUM(AA10:AB10)</f>
         <v>0.33303184704195105</v>
       </c>
     </row>
-    <row r="11" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O11" t="str">
         <f t="shared" si="0"/>
         <v>JAGUAR (0.18%)</v>
@@ -6190,8 +5300,17 @@
       <c r="T11" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+      <c r="U11">
+        <v>186</v>
+      </c>
+      <c r="V11">
+        <v>463</v>
+      </c>
+      <c r="W11">
+        <v>35246.533127889052</v>
+      </c>
+    </row>
+    <row r="12" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O12" t="str">
         <f t="shared" si="0"/>
         <v>SMART (0.19%)</v>
@@ -6212,15 +5331,24 @@
       <c r="T12" t="s">
         <v>74</v>
       </c>
-      <c r="X12" t="s">
+      <c r="U12">
+        <v>132</v>
+      </c>
+      <c r="V12">
+        <v>552</v>
+      </c>
+      <c r="W12">
+        <v>13713.450292397651</v>
+      </c>
+      <c r="AA12" t="s">
         <v>18</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="AB12" t="s">
         <v>17</v>
       </c>
-      <c r="Z12" s="3"/>
-    </row>
-    <row r="13" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC12" s="3"/>
+    </row>
+    <row r="13" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O13" t="str">
         <f t="shared" si="0"/>
         <v>HUMMER (0.22%)</v>
@@ -6241,21 +5369,30 @@
       <c r="T13" t="s">
         <v>49</v>
       </c>
-      <c r="W13" t="s">
+      <c r="U13">
+        <v>162</v>
+      </c>
+      <c r="V13">
+        <v>620</v>
+      </c>
+      <c r="W13">
+        <v>25166.240409207148</v>
+      </c>
+      <c r="Z13" t="s">
         <v>94</v>
       </c>
-      <c r="X13">
+      <c r="AA13">
         <v>180405</v>
       </c>
-      <c r="Y13">
+      <c r="AB13">
         <v>91161</v>
       </c>
-      <c r="Z13" s="3">
-        <f>Y13/SUM(X13:Y13)</f>
+      <c r="AC13" s="3">
+        <f>AB13/SUM(AA13:AB13)</f>
         <v>0.33568635248889772</v>
       </c>
     </row>
-    <row r="14" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O14" t="str">
         <f t="shared" si="0"/>
         <v>FIAT (0.22%)</v>
@@ -6276,21 +5413,30 @@
       <c r="T14" t="s">
         <v>44</v>
       </c>
-      <c r="W14" t="s">
+      <c r="U14">
+        <v>170</v>
+      </c>
+      <c r="V14">
+        <v>632</v>
+      </c>
+      <c r="W14">
+        <v>16926.43391521195</v>
+      </c>
+      <c r="Z14" t="s">
         <v>95</v>
       </c>
-      <c r="X14">
+      <c r="AA14">
         <v>57597</v>
       </c>
-      <c r="Y14">
+      <c r="AB14">
         <v>32393</v>
       </c>
-      <c r="Z14" s="3">
-        <f>Y14/SUM(X14:Y14)</f>
+      <c r="AC14" s="3">
+        <f>AB14/SUM(AA14:AB14)</f>
         <v>0.3599622180242249</v>
       </c>
     </row>
-    <row r="15" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O15" t="str">
         <f t="shared" si="0"/>
         <v>PORSCHE (0.29%)</v>
@@ -6311,8 +5457,17 @@
       <c r="T15" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="16" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+      <c r="U15">
+        <v>366</v>
+      </c>
+      <c r="V15">
+        <v>696</v>
+      </c>
+      <c r="W15">
+        <v>43705.273069679854</v>
+      </c>
+    </row>
+    <row r="16" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O16" t="str">
         <f t="shared" si="0"/>
         <v>LAND ROVER (0.30%)</v>
@@ -6333,8 +5488,17 @@
       <c r="T16" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+      <c r="U16">
+        <v>306</v>
+      </c>
+      <c r="V16">
+        <v>787</v>
+      </c>
+      <c r="W16">
+        <v>40274.473924977101</v>
+      </c>
+    </row>
+    <row r="17" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="O17" t="str">
         <f t="shared" si="0"/>
         <v>SUZUKI (0.37%)</v>
@@ -6355,17 +5519,26 @@
       <c r="T17" t="s">
         <v>76</v>
       </c>
-      <c r="W17" t="s">
+      <c r="U17">
+        <v>251</v>
+      </c>
+      <c r="V17">
+        <v>1069</v>
+      </c>
+      <c r="W17">
+        <v>15545.4545454545</v>
+      </c>
+      <c r="Z17" t="s">
         <v>96</v>
       </c>
-      <c r="X17" t="s">
+      <c r="AA17" t="s">
         <v>18</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="AB17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="O18" t="str">
         <f t="shared" si="0"/>
         <v>VOLVO (0.47%)</v>
@@ -6386,14 +5559,23 @@
       <c r="T18" t="s">
         <v>79</v>
       </c>
+      <c r="U18">
+        <v>557</v>
+      </c>
+      <c r="V18">
+        <v>1143</v>
+      </c>
       <c r="W18">
+        <v>22202.941176470551</v>
+      </c>
+      <c r="Z18">
         <v>1953</v>
       </c>
-      <c r="Y18">
+      <c r="AB18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="O19" t="str">
         <f t="shared" si="0"/>
         <v>MERCURY (0.50%)</v>
@@ -6414,14 +5596,23 @@
       <c r="T19" t="s">
         <v>63</v>
       </c>
+      <c r="U19">
+        <v>465</v>
+      </c>
+      <c r="V19">
+        <v>1336</v>
+      </c>
       <c r="W19">
+        <v>15247.084952803951</v>
+      </c>
+      <c r="Z19">
         <v>1963</v>
       </c>
-      <c r="X19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+      <c r="AA19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="O20" t="str">
         <f t="shared" si="0"/>
         <v>PONTIAC (0.57%)</v>
@@ -6442,17 +5633,26 @@
       <c r="T20" t="s">
         <v>69</v>
       </c>
+      <c r="U20">
+        <v>428</v>
+      </c>
+      <c r="V20">
+        <v>1650</v>
+      </c>
       <c r="W20">
+        <v>15810.8758421559</v>
+      </c>
+      <c r="Z20">
         <v>1966</v>
       </c>
-      <c r="X20">
-        <v>1</v>
-      </c>
-      <c r="Y20">
+      <c r="AA20">
+        <v>1</v>
+      </c>
+      <c r="AB20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="O21" t="str">
         <f t="shared" si="0"/>
         <v>SATURN (0.58%)</v>
@@ -6473,14 +5673,23 @@
       <c r="T21" t="s">
         <v>72</v>
       </c>
+      <c r="U21">
+        <v>403</v>
+      </c>
+      <c r="V21">
+        <v>1696</v>
+      </c>
       <c r="W21">
+        <v>14826.107670319199</v>
+      </c>
+      <c r="Z21">
         <v>1967</v>
       </c>
-      <c r="Y21">
+      <c r="AB21">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="O22" t="str">
         <f t="shared" si="0"/>
         <v>SCION (0.62%)</v>
@@ -6501,17 +5710,26 @@
       <c r="T22" t="s">
         <v>73</v>
       </c>
+      <c r="U22">
+        <v>423</v>
+      </c>
+      <c r="V22">
+        <v>1820</v>
+      </c>
       <c r="W22">
+        <v>16330.806954971</v>
+      </c>
+      <c r="Z22">
         <v>1969</v>
       </c>
-      <c r="X22">
-        <v>1</v>
-      </c>
-      <c r="Y22">
+      <c r="AA22">
+        <v>1</v>
+      </c>
+      <c r="AB22">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>21</v>
       </c>
@@ -6559,14 +5777,23 @@
       <c r="T23" t="s">
         <v>58</v>
       </c>
+      <c r="U23">
+        <v>815</v>
+      </c>
+      <c r="V23">
+        <v>2035</v>
+      </c>
       <c r="W23">
+        <v>24042.10526315785</v>
+      </c>
+      <c r="Z23">
         <v>1971</v>
       </c>
-      <c r="Y23">
+      <c r="AB23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>22</v>
       </c>
@@ -6595,8 +5822,8 @@
         <v>1022</v>
       </c>
       <c r="M24" s="3">
-        <f>K24/SUM(K24:L24)</f>
-        <v>0.65273530411145086</v>
+        <f>L24/SUM(K24:L24)</f>
+        <v>0.34726469588854908</v>
       </c>
       <c r="N24" s="3"/>
       <c r="O24" t="str">
@@ -6619,14 +5846,23 @@
       <c r="T24" t="s">
         <v>75</v>
       </c>
+      <c r="U24">
+        <v>966</v>
+      </c>
+      <c r="V24">
+        <v>1931</v>
+      </c>
       <c r="W24">
+        <v>21239.212978943699</v>
+      </c>
+      <c r="Z24">
         <v>1972</v>
       </c>
-      <c r="X24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+      <c r="AA24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>23</v>
       </c>
@@ -6655,8 +5891,8 @@
         <v>40775</v>
       </c>
       <c r="M25" s="3">
-        <f t="shared" ref="M25:M27" si="2">K25/SUM(K25:L25)</f>
-        <v>0.6640438329076378</v>
+        <f t="shared" ref="M25:M27" si="2">L25/SUM(K25:L25)</f>
+        <v>0.3359561670923622</v>
       </c>
       <c r="N25" s="3"/>
       <c r="O25" t="str">
@@ -6679,17 +5915,26 @@
       <c r="T25" t="s">
         <v>64</v>
       </c>
+      <c r="U25">
+        <v>707</v>
+      </c>
+      <c r="V25">
+        <v>2265</v>
+      </c>
       <c r="W25">
+        <v>20503.028263795401</v>
+      </c>
+      <c r="Z25">
         <v>1974</v>
       </c>
-      <c r="X25">
-        <v>1</v>
-      </c>
-      <c r="Y25">
+      <c r="AA25">
+        <v>1</v>
+      </c>
+      <c r="AB25">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>24</v>
       </c>
@@ -6719,7 +5964,7 @@
       </c>
       <c r="M26" s="3">
         <f t="shared" si="2"/>
-        <v>0.65793386937448883</v>
+        <v>0.34206613062551117</v>
       </c>
       <c r="N26" s="3"/>
       <c r="O26" t="str">
@@ -6742,14 +5987,23 @@
       <c r="T26" t="s">
         <v>65</v>
       </c>
+      <c r="U26">
+        <v>605</v>
+      </c>
+      <c r="V26">
+        <v>2437</v>
+      </c>
       <c r="W26">
+        <v>17133.464825772498</v>
+      </c>
+      <c r="Z26">
         <v>1975</v>
       </c>
-      <c r="Y26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+      <c r="AB26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>25</v>
       </c>
@@ -6779,7 +6033,7 @@
       </c>
       <c r="M27" s="3">
         <f t="shared" si="2"/>
-        <v>0.6455903082800466</v>
+        <v>0.3544096917199534</v>
       </c>
       <c r="N27" s="3"/>
       <c r="O27" t="str">
@@ -6802,17 +6056,26 @@
       <c r="T27" t="s">
         <v>34</v>
       </c>
+      <c r="U27">
+        <v>874</v>
+      </c>
+      <c r="V27">
+        <v>2313</v>
+      </c>
       <c r="W27">
+        <v>30963.288358958253</v>
+      </c>
+      <c r="Z27">
         <v>1976</v>
       </c>
-      <c r="X27">
-        <v>1</v>
-      </c>
-      <c r="Y27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+      <c r="AA27">
+        <v>1</v>
+      </c>
+      <c r="AB27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>26</v>
       </c>
@@ -6851,17 +6114,26 @@
       <c r="T28" t="s">
         <v>37</v>
       </c>
+      <c r="U28">
+        <v>862</v>
+      </c>
+      <c r="V28">
+        <v>2340</v>
+      </c>
       <c r="W28">
+        <v>21296.064959400352</v>
+      </c>
+      <c r="Z28">
         <v>1977</v>
       </c>
-      <c r="X28">
-        <v>1</v>
-      </c>
-      <c r="Y28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+      <c r="AA28">
+        <v>1</v>
+      </c>
+      <c r="AB28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>27</v>
       </c>
@@ -6909,17 +6181,26 @@
       <c r="T29" t="s">
         <v>38</v>
       </c>
+      <c r="U29">
+        <v>1251</v>
+      </c>
+      <c r="V29">
+        <v>3431</v>
+      </c>
       <c r="W29">
+        <v>28533.746262281049</v>
+      </c>
+      <c r="Z29">
         <v>1978</v>
       </c>
-      <c r="X29">
-        <v>1</v>
-      </c>
-      <c r="Y29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+      <c r="AA29">
+        <v>1</v>
+      </c>
+      <c r="AB29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>28</v>
       </c>
@@ -6967,17 +6248,26 @@
       <c r="T30" t="s">
         <v>33</v>
       </c>
+      <c r="U30">
+        <v>1222</v>
+      </c>
+      <c r="V30">
+        <v>3602</v>
+      </c>
       <c r="W30">
+        <v>23680.555555555547</v>
+      </c>
+      <c r="Z30">
         <v>1979</v>
       </c>
-      <c r="X30">
+      <c r="AA30">
         <v>2</v>
       </c>
-      <c r="Y30">
+      <c r="AB30">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>29</v>
       </c>
@@ -7025,14 +6315,23 @@
       <c r="T31" t="s">
         <v>47</v>
       </c>
+      <c r="U31">
+        <v>1443</v>
+      </c>
+      <c r="V31">
+        <v>4477</v>
+      </c>
       <c r="W31">
+        <v>25807.432432432397</v>
+      </c>
+      <c r="Z31">
         <v>1980</v>
       </c>
-      <c r="X31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+      <c r="AA31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>30</v>
       </c>
@@ -7077,14 +6376,23 @@
       <c r="T32" t="s">
         <v>51</v>
       </c>
+      <c r="U32">
+        <v>1677</v>
+      </c>
+      <c r="V32">
+        <v>5494</v>
+      </c>
       <c r="W32">
+        <v>26790.545251708249</v>
+      </c>
+      <c r="Z32">
         <v>1982</v>
       </c>
-      <c r="Y32">
+      <c r="AB32">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>31</v>
       </c>
@@ -7132,14 +6440,23 @@
       <c r="T33" t="s">
         <v>57</v>
       </c>
+      <c r="U33">
+        <v>2415</v>
+      </c>
+      <c r="V33">
+        <v>6814</v>
+      </c>
       <c r="W33">
+        <v>27107.487268393099</v>
+      </c>
+      <c r="Z33">
         <v>1983</v>
       </c>
-      <c r="Y33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+      <c r="AB33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>32</v>
       </c>
@@ -7184,14 +6501,23 @@
       <c r="T34" t="s">
         <v>55</v>
       </c>
+      <c r="U34">
+        <v>1858</v>
+      </c>
+      <c r="V34">
+        <v>7409</v>
+      </c>
       <c r="W34">
+        <v>18636.020287039999</v>
+      </c>
+      <c r="Z34">
         <v>1984</v>
       </c>
-      <c r="Y34">
+      <c r="AB34">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F35" t="s">
         <v>44</v>
       </c>
@@ -7230,17 +6556,26 @@
       <c r="T35" t="s">
         <v>40</v>
       </c>
+      <c r="U35">
+        <v>1993</v>
+      </c>
+      <c r="V35">
+        <v>7443</v>
+      </c>
       <c r="W35">
+        <v>19815.0699448919</v>
+      </c>
+      <c r="Z35">
         <v>1985</v>
       </c>
-      <c r="X35">
-        <v>1</v>
-      </c>
-      <c r="Y35">
+      <c r="AA35">
+        <v>1</v>
+      </c>
+      <c r="AB35">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F36" t="s">
         <v>45</v>
       </c>
@@ -7279,17 +6614,26 @@
       <c r="T36" t="s">
         <v>61</v>
       </c>
+      <c r="U36">
+        <v>2173</v>
+      </c>
+      <c r="V36">
+        <v>8120</v>
+      </c>
       <c r="W36">
+        <v>17820.84912076165</v>
+      </c>
+      <c r="Z36">
         <v>1986</v>
       </c>
-      <c r="X36">
+      <c r="AA36">
         <v>4</v>
       </c>
-      <c r="Y36">
+      <c r="AB36">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F37" t="s">
         <v>46</v>
       </c>
@@ -7328,17 +6672,26 @@
       <c r="T37" t="s">
         <v>62</v>
       </c>
+      <c r="U37">
+        <v>2510</v>
+      </c>
+      <c r="V37">
+        <v>8176</v>
+      </c>
       <c r="W37">
+        <v>31437.394722066249</v>
+      </c>
+      <c r="Z37">
         <v>1987</v>
       </c>
-      <c r="X37">
+      <c r="AA37">
         <v>4</v>
       </c>
-      <c r="Y37">
+      <c r="AB37">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F38" t="s">
         <v>47</v>
       </c>
@@ -7377,17 +6730,26 @@
       <c r="T38" t="s">
         <v>78</v>
       </c>
+      <c r="U38">
+        <v>2541</v>
+      </c>
+      <c r="V38">
+        <v>8180</v>
+      </c>
       <c r="W38">
+        <v>19999.067251189252</v>
+      </c>
+      <c r="Z38">
         <v>1988</v>
       </c>
-      <c r="X38">
+      <c r="AA38">
         <v>4</v>
       </c>
-      <c r="Y38">
+      <c r="AB38">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F39" t="s">
         <v>48</v>
       </c>
@@ -7426,17 +6788,26 @@
       <c r="T39" t="s">
         <v>36</v>
       </c>
+      <c r="U39">
+        <v>2710</v>
+      </c>
+      <c r="V39">
+        <v>8476</v>
+      </c>
       <c r="W39">
+        <v>29669.229393885202</v>
+      </c>
+      <c r="Z39">
         <v>1989</v>
       </c>
-      <c r="X39">
+      <c r="AA39">
         <v>13</v>
       </c>
-      <c r="Y39">
+      <c r="AB39">
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F40" t="s">
         <v>49</v>
       </c>
@@ -7475,17 +6846,26 @@
       <c r="T40" t="s">
         <v>54</v>
       </c>
+      <c r="U40">
+        <v>2957</v>
+      </c>
+      <c r="V40">
+        <v>8854</v>
+      </c>
       <c r="W40">
+        <v>21679.790026246701</v>
+      </c>
+      <c r="Z40">
         <v>1990</v>
       </c>
-      <c r="X40">
+      <c r="AA40">
         <v>7</v>
       </c>
-      <c r="Y40">
+      <c r="AB40">
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F41" t="s">
         <v>50</v>
       </c>
@@ -7524,17 +6904,26 @@
       <c r="T41" t="s">
         <v>50</v>
       </c>
+      <c r="U41">
+        <v>3040</v>
+      </c>
+      <c r="V41">
+        <v>11106</v>
+      </c>
       <c r="W41">
+        <v>18684.43376219425</v>
+      </c>
+      <c r="Z41">
         <v>1991</v>
       </c>
-      <c r="X41">
+      <c r="AA41">
         <v>14</v>
       </c>
-      <c r="Y41">
+      <c r="AB41">
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F42" t="s">
         <v>51</v>
       </c>
@@ -7573,17 +6962,26 @@
       <c r="T42" t="s">
         <v>42</v>
       </c>
+      <c r="U42">
+        <v>3986</v>
+      </c>
+      <c r="V42">
+        <v>16607</v>
+      </c>
       <c r="W42">
+        <v>20784.004273296749</v>
+      </c>
+      <c r="Z42">
         <v>1992</v>
       </c>
-      <c r="X42">
+      <c r="AA42">
         <v>25</v>
       </c>
-      <c r="Y42">
+      <c r="AB42">
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F43" t="s">
         <v>52</v>
       </c>
@@ -7622,17 +7020,26 @@
       <c r="T43" t="s">
         <v>48</v>
       </c>
+      <c r="U43">
+        <v>6989</v>
+      </c>
+      <c r="V43">
+        <v>20605</v>
+      </c>
       <c r="W43">
+        <v>19287.345075016299</v>
+      </c>
+      <c r="Z43">
         <v>1993</v>
       </c>
-      <c r="X43">
+      <c r="AA43">
         <v>26</v>
       </c>
-      <c r="Y43">
+      <c r="AB43">
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F44" t="s">
         <v>53</v>
       </c>
@@ -7671,17 +7078,26 @@
       <c r="T44" t="s">
         <v>39</v>
       </c>
+      <c r="U44">
+        <v>7412</v>
+      </c>
+      <c r="V44">
+        <v>30902</v>
+      </c>
       <c r="W44">
+        <v>20535.443963042202</v>
+      </c>
+      <c r="Z44">
         <v>1994</v>
       </c>
-      <c r="X44">
+      <c r="AA44">
         <v>35</v>
       </c>
-      <c r="Y44">
+      <c r="AB44">
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F45" t="s">
         <v>54</v>
       </c>
@@ -7720,17 +7136,26 @@
       <c r="T45" t="s">
         <v>66</v>
       </c>
+      <c r="U45">
+        <v>7716</v>
+      </c>
+      <c r="V45">
+        <v>31632</v>
+      </c>
       <c r="W45">
+        <v>19790.459489681798</v>
+      </c>
+      <c r="Z45">
         <v>1995</v>
       </c>
-      <c r="X45">
+      <c r="AA45">
         <v>45</v>
       </c>
-      <c r="Y45">
+      <c r="AB45">
         <v>105</v>
       </c>
     </row>
-    <row r="46" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F46" t="s">
         <v>55</v>
       </c>
@@ -7769,17 +7194,26 @@
       <c r="T46" t="s">
         <v>45</v>
       </c>
+      <c r="U46">
+        <v>10517</v>
+      </c>
+      <c r="V46">
+        <v>30228</v>
+      </c>
       <c r="W46">
+        <v>21175.84979752115</v>
+      </c>
+      <c r="Z46">
         <v>1996</v>
       </c>
-      <c r="X46">
+      <c r="AA46">
         <v>66</v>
       </c>
-      <c r="Y46">
+      <c r="AB46">
         <v>107</v>
       </c>
     </row>
-    <row r="47" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F47" t="s">
         <v>56</v>
       </c>
@@ -7818,17 +7252,26 @@
       <c r="T47" t="s">
         <v>77</v>
       </c>
+      <c r="U47">
+        <v>10830</v>
+      </c>
+      <c r="V47">
+        <v>30129</v>
+      </c>
       <c r="W47">
+        <v>20610.732683903399</v>
+      </c>
+      <c r="Z47">
         <v>1997</v>
       </c>
-      <c r="X47">
+      <c r="AA47">
         <v>85</v>
       </c>
-      <c r="Y47">
+      <c r="AB47">
         <v>173</v>
       </c>
     </row>
-    <row r="48" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F48" t="s">
         <v>57</v>
       </c>
@@ -7848,17 +7291,17 @@
         <v>3</v>
       </c>
       <c r="S48" s="5"/>
-      <c r="W48">
+      <c r="Z48">
         <v>1998</v>
       </c>
-      <c r="X48">
+      <c r="AA48">
         <v>121</v>
       </c>
-      <c r="Y48">
+      <c r="AB48">
         <v>232</v>
       </c>
     </row>
-    <row r="49" spans="6:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="49" spans="6:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F49" t="s">
         <v>58</v>
       </c>
@@ -7869,17 +7312,17 @@
         <v>1806</v>
       </c>
       <c r="S49" s="5"/>
-      <c r="W49">
+      <c r="Z49">
         <v>1999</v>
       </c>
-      <c r="X49">
+      <c r="AA49">
         <v>166</v>
       </c>
-      <c r="Y49">
+      <c r="AB49">
         <v>330</v>
       </c>
     </row>
-    <row r="50" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="50" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F50" t="s">
         <v>59</v>
       </c>
@@ -7913,17 +7356,17 @@
       <c r="T50" t="s">
         <v>17</v>
       </c>
-      <c r="W50">
+      <c r="Z50">
         <v>2000</v>
       </c>
-      <c r="X50">
+      <c r="AA50">
         <v>225</v>
       </c>
-      <c r="Y50">
+      <c r="AB50">
         <v>466</v>
       </c>
     </row>
-    <row r="51" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="51" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F51" t="s">
         <v>60</v>
       </c>
@@ -7957,17 +7400,17 @@
       <c r="T51">
         <v>1375</v>
       </c>
-      <c r="W51">
+      <c r="Z51">
         <v>2001</v>
       </c>
-      <c r="X51">
+      <c r="AA51">
         <v>252</v>
       </c>
-      <c r="Y51">
+      <c r="AB51">
         <v>456</v>
       </c>
     </row>
-    <row r="52" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="52" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F52" t="s">
         <v>61</v>
       </c>
@@ -8004,17 +7447,17 @@
       <c r="T52">
         <v>3338</v>
       </c>
-      <c r="W52">
+      <c r="Z52">
         <v>2002</v>
       </c>
-      <c r="X52">
+      <c r="AA52">
         <v>1382</v>
       </c>
-      <c r="Y52">
+      <c r="AB52">
         <v>1088</v>
       </c>
     </row>
-    <row r="53" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="53" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F53" t="s">
         <v>62</v>
       </c>
@@ -8051,17 +7494,17 @@
       <c r="T53">
         <v>33139</v>
       </c>
-      <c r="W53">
+      <c r="Z53">
         <v>2003</v>
       </c>
-      <c r="X53">
+      <c r="AA53">
         <v>3518</v>
       </c>
-      <c r="Y53">
+      <c r="AB53">
         <v>2130</v>
       </c>
     </row>
-    <row r="54" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="54" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F54" t="s">
         <v>63</v>
       </c>
@@ -8098,17 +7541,17 @@
       <c r="T54">
         <v>39374</v>
       </c>
-      <c r="W54">
+      <c r="Z54">
         <v>2004</v>
       </c>
-      <c r="X54">
+      <c r="AA54">
         <v>5637</v>
       </c>
-      <c r="Y54">
+      <c r="AB54">
         <v>3100</v>
       </c>
     </row>
-    <row r="55" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="55" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F55" t="s">
         <v>64</v>
       </c>
@@ -8145,17 +7588,17 @@
       <c r="T55">
         <v>32653</v>
       </c>
-      <c r="W55">
+      <c r="Z55">
         <v>2005</v>
       </c>
-      <c r="X55">
+      <c r="AA55">
         <v>8306</v>
       </c>
-      <c r="Y55">
+      <c r="AB55">
         <v>4453</v>
       </c>
     </row>
-    <row r="56" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="56" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F56" t="s">
         <v>65</v>
       </c>
@@ -8192,17 +7635,17 @@
       <c r="T56">
         <v>8828</v>
       </c>
-      <c r="W56">
+      <c r="Z56">
         <v>2006</v>
       </c>
-      <c r="X56">
+      <c r="AA56">
         <v>13387</v>
       </c>
-      <c r="Y56">
+      <c r="AB56">
         <v>7060</v>
       </c>
     </row>
-    <row r="57" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="57" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F57" t="s">
         <v>66</v>
       </c>
@@ -8239,17 +7682,17 @@
       <c r="T57">
         <v>3585</v>
       </c>
-      <c r="W57">
+      <c r="Z57">
         <v>2007</v>
       </c>
-      <c r="X57">
+      <c r="AA57">
         <v>19204</v>
       </c>
-      <c r="Y57">
+      <c r="AB57">
         <v>9837</v>
       </c>
     </row>
-    <row r="58" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="58" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F58" t="s">
         <v>67</v>
       </c>
@@ -8286,17 +7729,17 @@
       <c r="T58">
         <v>1262</v>
       </c>
-      <c r="W58">
+      <c r="Z58">
         <v>2008</v>
       </c>
-      <c r="X58">
+      <c r="AA58">
         <v>22247</v>
       </c>
-      <c r="Y58">
+      <c r="AB58">
         <v>11400</v>
       </c>
     </row>
-    <row r="59" spans="6:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="59" spans="6:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F59" t="s">
         <v>68</v>
       </c>
@@ -8325,17 +7768,17 @@
         <v>7958</v>
       </c>
       <c r="S59" s="5"/>
-      <c r="W59">
+      <c r="Z59">
         <v>2009</v>
       </c>
-      <c r="X59">
+      <c r="AA59">
         <v>19091</v>
       </c>
-      <c r="Y59">
+      <c r="AB59">
         <v>9768</v>
       </c>
     </row>
-    <row r="60" spans="6:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="60" spans="6:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F60" t="s">
         <v>69</v>
       </c>
@@ -8364,17 +7807,17 @@
         <v>7260</v>
       </c>
       <c r="S60" s="5"/>
-      <c r="W60">
+      <c r="Z60">
         <v>2010</v>
       </c>
-      <c r="X60">
+      <c r="AA60">
         <v>45687</v>
       </c>
-      <c r="Y60">
+      <c r="AB60">
         <v>22783</v>
       </c>
     </row>
-    <row r="61" spans="6:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="61" spans="6:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F61" t="s">
         <v>70</v>
       </c>
@@ -8394,17 +7837,17 @@
         <v>5891</v>
       </c>
       <c r="S61" s="5"/>
-      <c r="W61">
+      <c r="Z61">
         <v>2011</v>
       </c>
-      <c r="X61">
+      <c r="AA61">
         <v>40887</v>
       </c>
-      <c r="Y61">
+      <c r="AB61">
         <v>20406</v>
       </c>
     </row>
-    <row r="62" spans="6:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="62" spans="6:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F62" t="s">
         <v>71</v>
       </c>
@@ -8424,17 +7867,17 @@
         <v>5291</v>
       </c>
       <c r="S62" s="5"/>
-      <c r="W62">
+      <c r="Z62">
         <v>2012</v>
       </c>
-      <c r="X62">
+      <c r="AA62">
         <v>41639</v>
       </c>
-      <c r="Y62">
+      <c r="AB62">
         <v>21305</v>
       </c>
     </row>
-    <row r="63" spans="6:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="63" spans="6:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F63" t="s">
         <v>72</v>
       </c>
@@ -8454,17 +7897,17 @@
         <v>4503</v>
       </c>
       <c r="S63" s="5"/>
-      <c r="W63">
+      <c r="Z63">
         <v>2013</v>
       </c>
-      <c r="X63">
+      <c r="AA63">
         <v>15271</v>
       </c>
-      <c r="Y63">
+      <c r="AB63">
         <v>7758</v>
       </c>
     </row>
-    <row r="64" spans="6:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="64" spans="6:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F64" t="s">
         <v>73</v>
       </c>
@@ -8484,13 +7927,13 @@
         <v>3835</v>
       </c>
       <c r="S64" s="5"/>
-      <c r="W64">
+      <c r="Z64">
         <v>2014</v>
       </c>
-      <c r="X64">
+      <c r="AA64">
         <v>642</v>
       </c>
-      <c r="Y64">
+      <c r="AB64">
         <v>315</v>
       </c>
     </row>
@@ -12588,874 +12031,874 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="12" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="13" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="10" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="11">
         <v>0.38888888888888801</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>0.36783042394014898</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>0.32210834553440698</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="9">
         <v>0.36288998357963798</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="9">
         <v>0.32258064516128998</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="9">
         <v>0.33333333333333298</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="9">
         <v>0.35616438356164298</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="9">
         <v>0.27272727272727199</v>
       </c>
-      <c r="K3" s="14">
+      <c r="K3" s="11">
         <v>0.5</v>
       </c>
-      <c r="L3" s="14">
+      <c r="L3" s="11">
         <v>0.44444444444444398</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>0.367049808429118</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>0.33281855715591402</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>0.330718734219828</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="9">
         <v>0.34280422300426</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="9">
         <v>0.34169034486600902</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="9">
         <v>0.32338425381903602</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="9">
         <v>0.32095096582466498</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="9">
         <v>0.31640625</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="11">
         <v>0.41509433962264097</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L4" s="11">
         <v>0.45961002785515298</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>0.359837854692859</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>0.33837948252383099</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>0.34103177459302603</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>0.347936808419534</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="9">
         <v>0.34228814438336203</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="9">
         <v>0.33770585299778999</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="9">
         <v>0.31908704408145</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="9">
         <v>0.33600641539695197</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="9">
         <v>0.29670329670329598</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="11">
         <v>0.43768996960486301</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="11">
         <v>0.38073394495412799</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>0.35706554419723302</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>0.355103578154425</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <v>0.35471863367637302</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="9">
         <v>0.35162950257289799</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="9">
         <v>0.34274531730500402</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="9">
         <v>0.34994913530010102</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="9">
         <v>0.33495145631067902</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="9">
         <v>0.22222222222222199</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="11">
         <v>0.45652173913043398</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="12" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
     </row>
     <row r="9" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="13" t="s">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="K9" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="L9" s="10" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="13">
         <v>0.55681818181818099</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="13">
         <v>0.68226120857699801</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="13">
         <v>0.70350404312668402</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="13">
         <v>0.65909090909090895</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="13">
         <v>0.59799999999999998</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="13">
         <v>0.581395348837209</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10" s="13">
         <v>0.52</v>
       </c>
-      <c r="J10" s="17">
+      <c r="J10" s="14">
         <v>0.83333333333333304</v>
       </c>
-      <c r="K10" s="16">
+      <c r="K10" s="13">
         <v>0.57142857142857095</v>
       </c>
-      <c r="L10" s="17">
+      <c r="L10" s="14">
         <v>0.8</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="13" t="s">
+      <c r="A11" s="17"/>
+      <c r="B11" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="13">
         <v>0.36104513064132998</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="13">
         <v>0.36498229803669102</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="13">
         <v>0.40630712979890299</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="13">
         <v>0.39017808958445699</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="13">
         <v>0.36206896551724099</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="13">
         <v>0.34735202492211797</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="13">
         <v>0.27835051546391698</v>
       </c>
-      <c r="J11" s="16">
+      <c r="J11" s="13">
         <v>0.31578947368421001</v>
       </c>
-      <c r="K11" s="16">
+      <c r="K11" s="13">
         <v>0.15384615384615299</v>
       </c>
-      <c r="L11" s="17">
+      <c r="L11" s="14">
         <v>0.70270270270270196</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="13" t="s">
+      <c r="A12" s="17"/>
+      <c r="B12" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="13">
         <v>0.34461438333875599</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="13">
         <v>0.32666709126807197</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="13">
         <v>0.329936305732484</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="13">
         <v>0.34636205612118198</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12" s="13">
         <v>0.336808051761322</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="13">
         <v>0.329483282674772</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I12" s="13">
         <v>0.30674586338565901</v>
       </c>
-      <c r="J12" s="16">
+      <c r="J12" s="13">
         <v>0.33250620347394499</v>
       </c>
-      <c r="K12" s="16">
+      <c r="K12" s="13">
         <v>0.46938775510204001</v>
       </c>
-      <c r="L12" s="16">
+      <c r="L12" s="13">
         <v>0.375</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="13" t="s">
+      <c r="A13" s="17"/>
+      <c r="B13" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="13">
         <v>0.36906077348066202</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="13">
         <v>0.33072413914142301</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="13">
         <v>0.32932522755516702</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="13">
         <v>0.34289543264877298</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13" s="13">
         <v>0.33560664393355999</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="13">
         <v>0.3296011196641</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13" s="13">
         <v>0.33073206986250397</v>
       </c>
-      <c r="J13" s="16">
+      <c r="J13" s="13">
         <v>0.34168865435356199</v>
       </c>
-      <c r="K13" s="16">
+      <c r="K13" s="13">
         <v>0.217391304347826</v>
       </c>
-      <c r="L13" s="16">
+      <c r="L13" s="13">
         <v>0.42587601078167098</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="13" t="s">
+      <c r="A14" s="17"/>
+      <c r="B14" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="13">
         <v>0.37425742574257398</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="13">
         <v>0.33287460535902202</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="13">
         <v>0.33521876559640601</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="13">
         <v>0.33934388087482498</v>
       </c>
-      <c r="G14" s="16">
+      <c r="G14" s="13">
         <v>0.34313279330117402</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="13">
         <v>0.33103843947217398</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="13">
         <v>0.33355525965379401</v>
       </c>
-      <c r="J14" s="16">
+      <c r="J14" s="13">
         <v>0.28527607361963098</v>
       </c>
-      <c r="K14" s="16">
+      <c r="K14" s="13">
         <v>0.31818181818181801</v>
       </c>
-      <c r="L14" s="16">
+      <c r="L14" s="13">
         <v>0.44015444015444</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
-      <c r="B15" s="13" t="s">
+      <c r="A15" s="17"/>
+      <c r="B15" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="13">
         <v>0.41450777202072497</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="13">
         <v>0.336713138994507</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="13">
         <v>0.33691395322815199</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="13">
         <v>0.34367853642600399</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="13">
         <v>0.34658785599140202</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="13">
         <v>0.33854166666666602</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="13">
         <v>0.328125</v>
       </c>
-      <c r="J15" s="16">
+      <c r="J15" s="13">
         <v>0.31410256410256399</v>
       </c>
-      <c r="K15" s="16">
+      <c r="K15" s="13">
         <v>0.375</v>
       </c>
-      <c r="L15" s="16">
+      <c r="L15" s="13">
         <v>0.455696202531645</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
-      <c r="B16" s="13" t="s">
+      <c r="A16" s="17"/>
+      <c r="B16" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="13">
         <v>0.435294117647058</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="13">
         <v>0.34253246753246702</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="13">
         <v>0.33057471264367799</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="13">
         <v>0.341220698805838</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G16" s="13">
         <v>0.34807472359893199</v>
       </c>
-      <c r="H16" s="16">
+      <c r="H16" s="13">
         <v>0.32927756653992302</v>
       </c>
-      <c r="I16" s="16">
+      <c r="I16" s="13">
         <v>0.35127478753541003</v>
       </c>
-      <c r="J16" s="16">
+      <c r="J16" s="13">
         <v>0.32758620689655099</v>
       </c>
-      <c r="K16" s="16">
+      <c r="K16" s="13">
         <v>0.25</v>
       </c>
-      <c r="L16" s="16">
+      <c r="L16" s="13">
         <v>0.50892857142857095</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="13" t="s">
+      <c r="A17" s="17"/>
+      <c r="B17" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="13">
         <v>0.44827586206896503</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="13">
         <v>0.34788189987162998</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="13">
         <v>0.35380835380835302</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="13">
         <v>0.34663120567375799</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G17" s="13">
         <v>0.34398782343987799</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H17" s="13">
         <v>0.331738437001594</v>
       </c>
-      <c r="I17" s="16">
+      <c r="I17" s="13">
         <v>0.29936305732483998</v>
       </c>
-      <c r="J17" s="16">
+      <c r="J17" s="13">
         <v>0.25</v>
       </c>
-      <c r="K17" s="16">
+      <c r="K17" s="13">
         <v>0</v>
       </c>
-      <c r="L17" s="16">
+      <c r="L17" s="13">
         <v>0.31578947368421001</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="13" t="s">
+      <c r="A18" s="17"/>
+      <c r="B18" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="13">
         <v>0.45</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="13">
         <v>0.38095238095237999</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="13">
         <v>0.37041564792176002</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="13">
         <v>0.35122410546139299</v>
       </c>
-      <c r="G18" s="16">
+      <c r="G18" s="13">
         <v>0.38461538461538403</v>
       </c>
-      <c r="H18" s="16">
+      <c r="H18" s="13">
         <v>0.35199999999999998</v>
       </c>
-      <c r="I18" s="16">
+      <c r="I18" s="13">
         <v>0.4</v>
       </c>
-      <c r="J18" s="16">
+      <c r="J18" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="K18" s="16">
+      <c r="K18" s="13">
         <v>0</v>
       </c>
-      <c r="L18" s="16">
+      <c r="L18" s="13">
         <v>0.54545454545454497</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="13" t="s">
+      <c r="A19" s="17"/>
+      <c r="B19" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="13">
         <v>0.26315789473684198</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="13">
         <v>0.34146341463414598</v>
       </c>
-      <c r="E19" s="16">
+      <c r="E19" s="13">
         <v>0.40570175438596401</v>
       </c>
-      <c r="F19" s="16">
+      <c r="F19" s="13">
         <v>0.375494071146245</v>
       </c>
-      <c r="G19" s="16">
+      <c r="G19" s="13">
         <v>0.34732824427480902</v>
       </c>
-      <c r="H19" s="16">
+      <c r="H19" s="13">
         <v>0.369747899159663</v>
       </c>
-      <c r="I19" s="16">
+      <c r="I19" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="J19" s="16">
+      <c r="J19" s="13">
         <v>0.25</v>
       </c>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16">
+      <c r="K19" s="13"/>
+      <c r="L19" s="13">
         <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
-      <c r="B20" s="13" t="s">
+      <c r="A20" s="17"/>
+      <c r="B20" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20" s="13">
         <v>0.14285714285714199</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="13">
         <v>0.38983050847457601</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="13">
         <v>0.38725490196078399</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F20" s="13">
         <v>0.34146341463414598</v>
       </c>
-      <c r="G20" s="16">
+      <c r="G20" s="13">
         <v>0.41489361702127597</v>
       </c>
-      <c r="H20" s="16">
+      <c r="H20" s="13">
         <v>0.37254901960784298</v>
       </c>
-      <c r="I20" s="16">
+      <c r="I20" s="13">
         <v>0.214285714285714</v>
       </c>
-      <c r="J20" s="16">
+      <c r="J20" s="13">
         <v>0</v>
       </c>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16">
+      <c r="K20" s="13"/>
+      <c r="L20" s="13">
         <v>0.2</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="11"/>
-      <c r="B21" s="13" t="s">
+      <c r="A21" s="17"/>
+      <c r="B21" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="13">
         <v>0.57499999999999996</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="13">
         <v>0.37962962962962898</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F21" s="13">
         <v>0.34166666666666601</v>
       </c>
-      <c r="G21" s="16">
+      <c r="G21" s="13">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H21" s="16">
+      <c r="H21" s="13">
         <v>0.47058823529411697</v>
       </c>
-      <c r="I21" s="16">
+      <c r="I21" s="13">
         <v>0.22222222222222199</v>
       </c>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16">
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13">
         <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
-      <c r="B22" s="13" t="s">
+      <c r="A22" s="17"/>
+      <c r="B22" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C22" s="16">
+      <c r="C22" s="13">
         <v>0.5</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="13">
         <v>0.56666666666666599</v>
       </c>
-      <c r="E22" s="16">
+      <c r="E22" s="13">
         <v>0.5</v>
       </c>
-      <c r="F22" s="16">
+      <c r="F22" s="13">
         <v>0.36065573770491799</v>
       </c>
-      <c r="G22" s="16">
+      <c r="G22" s="13">
         <v>0.46875</v>
       </c>
-      <c r="H22" s="16">
+      <c r="H22" s="13">
         <v>0.52631578947368396</v>
       </c>
-      <c r="I22" s="16">
+      <c r="I22" s="13">
         <v>0.42857142857142799</v>
       </c>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="17">
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
-      <c r="B23" s="13" t="s">
+      <c r="A23" s="17"/>
+      <c r="B23" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16">
+      <c r="C23" s="13"/>
+      <c r="D23" s="13">
         <v>0.46153846153846101</v>
       </c>
-      <c r="E23" s="16">
+      <c r="E23" s="13">
         <v>0.40540540540540498</v>
       </c>
-      <c r="F23" s="16">
+      <c r="F23" s="13">
         <v>0.4</v>
       </c>
-      <c r="G23" s="16">
+      <c r="G23" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="H23" s="16">
+      <c r="H23" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="I23" s="17">
-        <v>1</v>
-      </c>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16">
+      <c r="I23" s="14">
+        <v>1</v>
+      </c>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
-      <c r="B24" s="13" t="s">
+      <c r="A24" s="17"/>
+      <c r="B24" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="16">
+      <c r="C24" s="15"/>
+      <c r="D24" s="13">
         <v>0.42857142857142799</v>
       </c>
-      <c r="E24" s="16">
+      <c r="E24" s="13">
         <v>0.5625</v>
       </c>
-      <c r="F24" s="16">
+      <c r="F24" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="G24" s="16">
+      <c r="G24" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="H24" s="16">
+      <c r="H24" s="13">
         <v>0.25</v>
       </c>
-      <c r="I24" s="16">
+      <c r="I24" s="13">
         <v>0</v>
       </c>
-      <c r="J24" s="17">
-        <v>1</v>
-      </c>
-      <c r="K24" s="18"/>
-      <c r="L24" s="16">
+      <c r="J24" s="14">
+        <v>1</v>
+      </c>
+      <c r="K24" s="15"/>
+      <c r="L24" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
-      <c r="B25" s="13" t="s">
+      <c r="A25" s="17"/>
+      <c r="B25" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="16">
+      <c r="C25" s="15"/>
+      <c r="D25" s="13">
         <v>0.5</v>
       </c>
-      <c r="E25" s="16">
+      <c r="E25" s="13">
         <v>0.5</v>
       </c>
-      <c r="F25" s="16">
+      <c r="F25" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="G25" s="17">
+      <c r="G25" s="14">
         <v>0.8</v>
       </c>
-      <c r="H25" s="16">
+      <c r="H25" s="13">
         <v>0.6</v>
       </c>
-      <c r="I25" s="16">
+      <c r="I25" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="16">
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="11"/>
-      <c r="B26" s="13" t="s">
+      <c r="A26" s="17"/>
+      <c r="B26" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="17">
-        <v>1</v>
-      </c>
-      <c r="E26" s="16">
+      <c r="C26" s="15"/>
+      <c r="D26" s="14">
+        <v>1</v>
+      </c>
+      <c r="E26" s="13">
         <v>0</v>
       </c>
-      <c r="F26" s="16">
+      <c r="F26" s="13">
         <v>0.28571428571428498</v>
       </c>
-      <c r="G26" s="17">
+      <c r="G26" s="14">
         <v>0.66666666666666596</v>
       </c>
-      <c r="H26" s="16">
+      <c r="H26" s="13">
         <v>0.5</v>
       </c>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
     </row>
     <row r="27" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="11"/>
-      <c r="B27" s="13" t="s">
+      <c r="A27" s="17"/>
+      <c r="B27" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="16">
+      <c r="C27" s="15"/>
+      <c r="D27" s="13">
         <v>0</v>
       </c>
-      <c r="E27" s="16">
+      <c r="E27" s="13">
         <v>0.25</v>
       </c>
-      <c r="F27" s="16">
+      <c r="F27" s="13">
         <v>0.16666666666666599</v>
       </c>
-      <c r="G27" s="16">
+      <c r="G27" s="13">
         <v>0.5</v>
       </c>
-      <c r="H27" s="18"/>
-      <c r="I27" s="16">
+      <c r="H27" s="15"/>
+      <c r="I27" s="13">
         <v>0.5</v>
       </c>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
     </row>
     <row r="28" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="11"/>
-      <c r="B28" s="13" t="s">
+      <c r="A28" s="17"/>
+      <c r="B28" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="17">
-        <v>1</v>
-      </c>
-      <c r="F28" s="16">
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="14">
+        <v>1</v>
+      </c>
+      <c r="F28" s="13">
         <v>0</v>
       </c>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="17">
-        <v>1</v>
-      </c>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="14">
+        <v>1</v>
+      </c>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -13528,7 +12971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2808B69F-E6D1-480C-BA78-6E297A9A26C0}">
   <dimension ref="B2:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -13538,10 +12981,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="18"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -13555,7 +12998,7 @@
       <c r="B4" t="s">
         <v>144</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="12">
         <v>11869.8570989203</v>
       </c>
     </row>
@@ -13563,7 +13006,7 @@
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="12">
         <v>1093.4368310766699</v>
       </c>
     </row>
@@ -13571,7 +13014,7 @@
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="12">
         <v>698.34771364557605</v>
       </c>
     </row>
@@ -13579,7 +13022,7 @@
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="12">
         <v>365.45830508648402</v>
       </c>
     </row>
@@ -13587,7 +13030,7 @@
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="12">
         <v>349.23024765668498</v>
       </c>
     </row>
@@ -13595,7 +13038,7 @@
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="12">
         <v>133.00166341609301</v>
       </c>
     </row>
@@ -13603,7 +13046,7 @@
       <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="12">
         <v>93.305188392097094</v>
       </c>
     </row>
@@ -13611,7 +13054,7 @@
       <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="12">
         <v>82.105560753168803</v>
       </c>
     </row>
@@ -13619,7 +13062,7 @@
       <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="12">
         <v>59.257995713963297</v>
       </c>
     </row>
@@ -13627,7 +13070,7 @@
       <c r="B13" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="12">
         <v>23.737361633894398</v>
       </c>
     </row>
@@ -13635,7 +13078,7 @@
       <c r="B14" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="12">
         <v>23.371714450063401</v>
       </c>
     </row>
@@ -13643,7 +13086,7 @@
       <c r="B15" t="s">
         <v>138</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="12">
         <v>7.3364809482583802</v>
       </c>
     </row>
@@ -13651,7 +13094,7 @@
       <c r="B16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="12">
         <v>2.0510437406890598</v>
       </c>
     </row>
@@ -13659,7 +13102,7 @@
       <c r="B17" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="12">
         <v>0.73113998038038097</v>
       </c>
     </row>
@@ -13667,7 +13110,7 @@
       <c r="B18" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="12">
         <v>0.21377281914893501</v>
       </c>
     </row>

</xml_diff>

<commit_message>
nothing of major importance
</commit_message>
<xml_diff>
--- a/regressor and classifier importances.xlsx
+++ b/regressor and classifier importances.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minna\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a38cc7a04266740c/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="389" documentId="8_{E93A6E45-9447-44B2-A386-D641E629DBB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0C4DF848-B10D-4A38-A3B4-226DB8C321D8}"/>
+  <xr:revisionPtr revIDLastSave="435" documentId="8_{E93A6E45-9447-44B2-A386-D641E629DBB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EE6DDEE8-17E3-438D-B0AD-9C9C87EFEE5C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{789FB943-771A-4B19-9A66-979F3CA78A6C}"/>
+    <workbookView xWindow="3552" yWindow="1200" windowWidth="13668" windowHeight="4500" firstSheet="1" activeTab="1" xr2:uid="{789FB943-771A-4B19-9A66-979F3CA78A6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Original Importances" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="Heatmaps" sheetId="3" r:id="rId3"/>
     <sheet name="chi - 2" sheetId="4" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="147">
   <si>
     <t>Classifier Importances</t>
   </si>
@@ -485,8 +488,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000%"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -567,34 +570,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1903,396 +1906,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Trade-In</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="percentStacked"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Distribution Data Tables (mess)'!$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Loyal</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Distribution Data Tables (mess)'!$G$2:$G$3</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Trade-In</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>No Trade-In</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Distribution Data Tables (mess)'!$I$2:$I$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>61077</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>62477</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FF9D-49F0-82BE-0652835F1EBF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Distribution Data Tables (mess)'!$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Nonloyal</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Distribution Data Tables (mess)'!$G$2:$G$3</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Trade-In</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>No Trade-In</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Distribution Data Tables (mess)'!$H$2:$H$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>106782</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>131220</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-FF9D-49F0-82BE-0652835F1EBF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
-        <c:axId val="2010917280"/>
-        <c:axId val="2015821296"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2010917280"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2015821296"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2015821296"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2010917280"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2414,46 +2027,6 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4513,511 +4086,6 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -5169,45 +4237,20 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78A77B9E-82EA-48F6-AA0D-83D0E2D0ECEC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5832,10 +4875,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58B855E-757F-44CC-B7FE-FF60EBDD6187}">
-  <dimension ref="B1:Z474"/>
+  <dimension ref="B1:AC474"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30:J48"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5843,7 +4886,7 @@
     <col min="15" max="15" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:29" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>18</v>
       </c>
@@ -5857,7 +4900,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>15</v>
       </c>
@@ -5872,16 +4915,16 @@
         <v>0.38706849171661128</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2">
-        <v>106782</v>
+        <v>131220</v>
       </c>
       <c r="I2">
-        <v>61077</v>
+        <v>62477</v>
       </c>
       <c r="J2" s="3">
-        <f>I2/SUM(H2:I2)</f>
+        <f>I3/SUM(H3:I3)</f>
         <v>0.36385895304988114</v>
       </c>
       <c r="P2" t="s">
@@ -5893,8 +4936,17 @@
       <c r="R2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+      <c r="U2" t="s">
+        <v>92</v>
+      </c>
+      <c r="V2" t="s">
+        <v>93</v>
+      </c>
+      <c r="W2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -5909,16 +4961,16 @@
         <v>0.32957725732803062</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3">
-        <v>131220</v>
+        <v>106782</v>
       </c>
       <c r="I3">
-        <v>62477</v>
+        <v>61077</v>
       </c>
       <c r="J3" s="3">
-        <f>I3/SUM(H3:I3)</f>
+        <f>I2/SUM(H2:I2)</f>
         <v>0.32255016856223895</v>
       </c>
       <c r="M3" t="s">
@@ -5944,12 +4996,22 @@
       <c r="T3" t="s">
         <v>87</v>
       </c>
-      <c r="W3" s="6">
+      <c r="U3">
+        <v>2</v>
+      </c>
+      <c r="W3">
+        <v>5000</v>
+      </c>
+      <c r="Y3">
+        <f>SUM(V3:V47)/SUM(U3:V47)</f>
+        <v>0.76755468032614593</v>
+      </c>
+      <c r="Z3" s="6">
         <f>SUM(R3:R47)/(SUM(Q3:Q47)+SUM(R3:R47))</f>
         <v>0.34172852891391653</v>
       </c>
     </row>
-    <row r="4" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O4" t="str">
         <f t="shared" ref="O4:O47" si="0">T4&amp;" ("&amp;S4&amp;")"</f>
         <v>BENTLEY/MASERATI (0.00%)</v>
@@ -5970,14 +5032,20 @@
       <c r="T4" t="s">
         <v>88</v>
       </c>
-      <c r="X4" t="s">
+      <c r="U4">
+        <v>4</v>
+      </c>
+      <c r="W4">
+        <v>57500</v>
+      </c>
+      <c r="AA4" t="s">
         <v>18</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AB4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O5" t="str">
         <f t="shared" si="0"/>
         <v>LOTUS (0.00%)</v>
@@ -5998,21 +5066,27 @@
       <c r="T5" t="s">
         <v>59</v>
       </c>
-      <c r="W5" t="s">
+      <c r="U5">
+        <v>4</v>
+      </c>
+      <c r="W5">
+        <v>23750</v>
+      </c>
+      <c r="Z5" t="s">
         <v>90</v>
       </c>
-      <c r="X5">
+      <c r="AA5">
         <v>146486</v>
       </c>
-      <c r="Y5">
+      <c r="AB5">
         <v>78098</v>
       </c>
-      <c r="Z5" s="3">
-        <f>Y5/SUM(X5:Y5)</f>
+      <c r="AC5" s="3">
+        <f>AB5/SUM(AA5:AB5)</f>
         <v>0.34774516439283298</v>
       </c>
     </row>
-    <row r="6" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O6" t="str">
         <f t="shared" si="0"/>
         <v>PLYMOUTH (0.00%)</v>
@@ -6033,21 +5107,27 @@
       <c r="T6" t="s">
         <v>68</v>
       </c>
-      <c r="W6" t="s">
+      <c r="U6">
+        <v>8</v>
+      </c>
+      <c r="W6">
+        <v>5000</v>
+      </c>
+      <c r="Z6" t="s">
         <v>91</v>
       </c>
-      <c r="X6">
+      <c r="AA6">
         <v>91516</v>
       </c>
-      <c r="Y6">
+      <c r="AB6">
         <v>45456</v>
       </c>
-      <c r="Z6" s="3">
-        <f>Y6/SUM(X6:Y6)</f>
+      <c r="AC6" s="3">
+        <f>AB6/SUM(AA6:AB6)</f>
         <v>0.33186344654381916</v>
       </c>
     </row>
-    <row r="7" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O7" t="str">
         <f t="shared" si="0"/>
         <v>GEO (0.00%)</v>
@@ -6068,9 +5148,15 @@
       <c r="T7" t="s">
         <v>46</v>
       </c>
-      <c r="Z7" s="3"/>
-    </row>
-    <row r="8" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+      <c r="U7">
+        <v>12</v>
+      </c>
+      <c r="W7">
+        <v>5000</v>
+      </c>
+      <c r="AC7" s="3"/>
+    </row>
+    <row r="8" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O8" t="str">
         <f t="shared" si="0"/>
         <v>SAAB (0.01%)</v>
@@ -6091,15 +5177,21 @@
       <c r="T8" t="s">
         <v>71</v>
       </c>
-      <c r="X8" t="s">
+      <c r="U8">
+        <v>25</v>
+      </c>
+      <c r="W8">
+        <v>7400</v>
+      </c>
+      <c r="AA8" t="s">
         <v>18</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="AB8" t="s">
         <v>17</v>
       </c>
-      <c r="Z8" s="3"/>
-    </row>
-    <row r="9" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC8" s="3"/>
+    </row>
+    <row r="9" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O9" t="str">
         <f t="shared" si="0"/>
         <v>OLDSMOBILE (0.01%)</v>
@@ -6120,21 +5212,30 @@
       <c r="T9" t="s">
         <v>67</v>
       </c>
-      <c r="W9" t="s">
+      <c r="U9">
+        <v>39</v>
+      </c>
+      <c r="V9">
+        <v>8</v>
+      </c>
+      <c r="W9">
+        <v>6276.5957446808497</v>
+      </c>
+      <c r="Z9" t="s">
         <v>92</v>
       </c>
-      <c r="X9">
+      <c r="AA9">
         <v>52909</v>
       </c>
-      <c r="Y9">
+      <c r="AB9">
         <v>31133</v>
       </c>
-      <c r="Z9" s="3">
-        <f>Y9/SUM(X9:Y9)</f>
+      <c r="AC9" s="3">
+        <f>AB9/SUM(AA9:AB9)</f>
         <v>0.37044572951619431</v>
       </c>
     </row>
-    <row r="10" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O10" t="str">
         <f t="shared" si="0"/>
         <v>ISUZU (0.02%)</v>
@@ -6155,21 +5256,30 @@
       <c r="T10" t="s">
         <v>52</v>
       </c>
-      <c r="W10" t="s">
+      <c r="U10">
+        <v>30</v>
+      </c>
+      <c r="V10">
+        <v>36</v>
+      </c>
+      <c r="W10">
+        <v>10984.848484848451</v>
+      </c>
+      <c r="Z10" t="s">
         <v>93</v>
       </c>
-      <c r="X10">
+      <c r="AA10">
         <v>185093</v>
       </c>
-      <c r="Y10">
+      <c r="AB10">
         <v>92421</v>
       </c>
-      <c r="Z10" s="3">
-        <f>Y10/SUM(X10:Y10)</f>
+      <c r="AC10" s="3">
+        <f>AB10/SUM(AA10:AB10)</f>
         <v>0.33303184704195105</v>
       </c>
     </row>
-    <row r="11" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O11" t="str">
         <f t="shared" si="0"/>
         <v>JAGUAR (0.18%)</v>
@@ -6190,8 +5300,17 @@
       <c r="T11" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+      <c r="U11">
+        <v>186</v>
+      </c>
+      <c r="V11">
+        <v>463</v>
+      </c>
+      <c r="W11">
+        <v>35246.533127889052</v>
+      </c>
+    </row>
+    <row r="12" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O12" t="str">
         <f t="shared" si="0"/>
         <v>SMART (0.19%)</v>
@@ -6212,15 +5331,24 @@
       <c r="T12" t="s">
         <v>74</v>
       </c>
-      <c r="X12" t="s">
+      <c r="U12">
+        <v>132</v>
+      </c>
+      <c r="V12">
+        <v>552</v>
+      </c>
+      <c r="W12">
+        <v>13713.450292397651</v>
+      </c>
+      <c r="AA12" t="s">
         <v>18</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="AB12" t="s">
         <v>17</v>
       </c>
-      <c r="Z12" s="3"/>
-    </row>
-    <row r="13" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC12" s="3"/>
+    </row>
+    <row r="13" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O13" t="str">
         <f t="shared" si="0"/>
         <v>HUMMER (0.22%)</v>
@@ -6241,21 +5369,30 @@
       <c r="T13" t="s">
         <v>49</v>
       </c>
-      <c r="W13" t="s">
+      <c r="U13">
+        <v>162</v>
+      </c>
+      <c r="V13">
+        <v>620</v>
+      </c>
+      <c r="W13">
+        <v>25166.240409207148</v>
+      </c>
+      <c r="Z13" t="s">
         <v>94</v>
       </c>
-      <c r="X13">
+      <c r="AA13">
         <v>180405</v>
       </c>
-      <c r="Y13">
+      <c r="AB13">
         <v>91161</v>
       </c>
-      <c r="Z13" s="3">
-        <f>Y13/SUM(X13:Y13)</f>
+      <c r="AC13" s="3">
+        <f>AB13/SUM(AA13:AB13)</f>
         <v>0.33568635248889772</v>
       </c>
     </row>
-    <row r="14" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O14" t="str">
         <f t="shared" si="0"/>
         <v>FIAT (0.22%)</v>
@@ -6276,21 +5413,30 @@
       <c r="T14" t="s">
         <v>44</v>
       </c>
-      <c r="W14" t="s">
+      <c r="U14">
+        <v>170</v>
+      </c>
+      <c r="V14">
+        <v>632</v>
+      </c>
+      <c r="W14">
+        <v>16926.43391521195</v>
+      </c>
+      <c r="Z14" t="s">
         <v>95</v>
       </c>
-      <c r="X14">
+      <c r="AA14">
         <v>57597</v>
       </c>
-      <c r="Y14">
+      <c r="AB14">
         <v>32393</v>
       </c>
-      <c r="Z14" s="3">
-        <f>Y14/SUM(X14:Y14)</f>
+      <c r="AC14" s="3">
+        <f>AB14/SUM(AA14:AB14)</f>
         <v>0.3599622180242249</v>
       </c>
     </row>
-    <row r="15" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O15" t="str">
         <f t="shared" si="0"/>
         <v>PORSCHE (0.29%)</v>
@@ -6311,8 +5457,17 @@
       <c r="T15" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="16" spans="2:26" ht="15" x14ac:dyDescent="0.35">
+      <c r="U15">
+        <v>366</v>
+      </c>
+      <c r="V15">
+        <v>696</v>
+      </c>
+      <c r="W15">
+        <v>43705.273069679854</v>
+      </c>
+    </row>
+    <row r="16" spans="2:29" ht="15" x14ac:dyDescent="0.35">
       <c r="O16" t="str">
         <f t="shared" si="0"/>
         <v>LAND ROVER (0.30%)</v>
@@ -6333,8 +5488,17 @@
       <c r="T16" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+      <c r="U16">
+        <v>306</v>
+      </c>
+      <c r="V16">
+        <v>787</v>
+      </c>
+      <c r="W16">
+        <v>40274.473924977101</v>
+      </c>
+    </row>
+    <row r="17" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="O17" t="str">
         <f t="shared" si="0"/>
         <v>SUZUKI (0.37%)</v>
@@ -6355,17 +5519,26 @@
       <c r="T17" t="s">
         <v>76</v>
       </c>
-      <c r="W17" t="s">
+      <c r="U17">
+        <v>251</v>
+      </c>
+      <c r="V17">
+        <v>1069</v>
+      </c>
+      <c r="W17">
+        <v>15545.4545454545</v>
+      </c>
+      <c r="Z17" t="s">
         <v>96</v>
       </c>
-      <c r="X17" t="s">
+      <c r="AA17" t="s">
         <v>18</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="AB17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="O18" t="str">
         <f t="shared" si="0"/>
         <v>VOLVO (0.47%)</v>
@@ -6386,14 +5559,23 @@
       <c r="T18" t="s">
         <v>79</v>
       </c>
+      <c r="U18">
+        <v>557</v>
+      </c>
+      <c r="V18">
+        <v>1143</v>
+      </c>
       <c r="W18">
+        <v>22202.941176470551</v>
+      </c>
+      <c r="Z18">
         <v>1953</v>
       </c>
-      <c r="Y18">
+      <c r="AB18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="O19" t="str">
         <f t="shared" si="0"/>
         <v>MERCURY (0.50%)</v>
@@ -6414,14 +5596,23 @@
       <c r="T19" t="s">
         <v>63</v>
       </c>
+      <c r="U19">
+        <v>465</v>
+      </c>
+      <c r="V19">
+        <v>1336</v>
+      </c>
       <c r="W19">
+        <v>15247.084952803951</v>
+      </c>
+      <c r="Z19">
         <v>1963</v>
       </c>
-      <c r="X19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+      <c r="AA19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="O20" t="str">
         <f t="shared" si="0"/>
         <v>PONTIAC (0.57%)</v>
@@ -6442,17 +5633,26 @@
       <c r="T20" t="s">
         <v>69</v>
       </c>
+      <c r="U20">
+        <v>428</v>
+      </c>
+      <c r="V20">
+        <v>1650</v>
+      </c>
       <c r="W20">
+        <v>15810.8758421559</v>
+      </c>
+      <c r="Z20">
         <v>1966</v>
       </c>
-      <c r="X20">
-        <v>1</v>
-      </c>
-      <c r="Y20">
+      <c r="AA20">
+        <v>1</v>
+      </c>
+      <c r="AB20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="O21" t="str">
         <f t="shared" si="0"/>
         <v>SATURN (0.58%)</v>
@@ -6473,14 +5673,23 @@
       <c r="T21" t="s">
         <v>72</v>
       </c>
+      <c r="U21">
+        <v>403</v>
+      </c>
+      <c r="V21">
+        <v>1696</v>
+      </c>
       <c r="W21">
+        <v>14826.107670319199</v>
+      </c>
+      <c r="Z21">
         <v>1967</v>
       </c>
-      <c r="Y21">
+      <c r="AB21">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="O22" t="str">
         <f t="shared" si="0"/>
         <v>SCION (0.62%)</v>
@@ -6501,17 +5710,26 @@
       <c r="T22" t="s">
         <v>73</v>
       </c>
+      <c r="U22">
+        <v>423</v>
+      </c>
+      <c r="V22">
+        <v>1820</v>
+      </c>
       <c r="W22">
+        <v>16330.806954971</v>
+      </c>
+      <c r="Z22">
         <v>1969</v>
       </c>
-      <c r="X22">
-        <v>1</v>
-      </c>
-      <c r="Y22">
+      <c r="AA22">
+        <v>1</v>
+      </c>
+      <c r="AB22">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>21</v>
       </c>
@@ -6559,14 +5777,23 @@
       <c r="T23" t="s">
         <v>58</v>
       </c>
+      <c r="U23">
+        <v>815</v>
+      </c>
+      <c r="V23">
+        <v>2035</v>
+      </c>
       <c r="W23">
+        <v>24042.10526315785</v>
+      </c>
+      <c r="Z23">
         <v>1971</v>
       </c>
-      <c r="Y23">
+      <c r="AB23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>22</v>
       </c>
@@ -6595,8 +5822,8 @@
         <v>1022</v>
       </c>
       <c r="M24" s="3">
-        <f>K24/SUM(K24:L24)</f>
-        <v>0.65273530411145086</v>
+        <f>L24/SUM(K24:L24)</f>
+        <v>0.34726469588854908</v>
       </c>
       <c r="N24" s="3"/>
       <c r="O24" t="str">
@@ -6619,14 +5846,23 @@
       <c r="T24" t="s">
         <v>75</v>
       </c>
+      <c r="U24">
+        <v>966</v>
+      </c>
+      <c r="V24">
+        <v>1931</v>
+      </c>
       <c r="W24">
+        <v>21239.212978943699</v>
+      </c>
+      <c r="Z24">
         <v>1972</v>
       </c>
-      <c r="X24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+      <c r="AA24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>23</v>
       </c>
@@ -6655,8 +5891,8 @@
         <v>40775</v>
       </c>
       <c r="M25" s="3">
-        <f t="shared" ref="M25:M27" si="2">K25/SUM(K25:L25)</f>
-        <v>0.6640438329076378</v>
+        <f t="shared" ref="M25:M27" si="2">L25/SUM(K25:L25)</f>
+        <v>0.3359561670923622</v>
       </c>
       <c r="N25" s="3"/>
       <c r="O25" t="str">
@@ -6679,17 +5915,26 @@
       <c r="T25" t="s">
         <v>64</v>
       </c>
+      <c r="U25">
+        <v>707</v>
+      </c>
+      <c r="V25">
+        <v>2265</v>
+      </c>
       <c r="W25">
+        <v>20503.028263795401</v>
+      </c>
+      <c r="Z25">
         <v>1974</v>
       </c>
-      <c r="X25">
-        <v>1</v>
-      </c>
-      <c r="Y25">
+      <c r="AA25">
+        <v>1</v>
+      </c>
+      <c r="AB25">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>24</v>
       </c>
@@ -6719,7 +5964,7 @@
       </c>
       <c r="M26" s="3">
         <f t="shared" si="2"/>
-        <v>0.65793386937448883</v>
+        <v>0.34206613062551117</v>
       </c>
       <c r="N26" s="3"/>
       <c r="O26" t="str">
@@ -6742,14 +5987,23 @@
       <c r="T26" t="s">
         <v>65</v>
       </c>
+      <c r="U26">
+        <v>605</v>
+      </c>
+      <c r="V26">
+        <v>2437</v>
+      </c>
       <c r="W26">
+        <v>17133.464825772498</v>
+      </c>
+      <c r="Z26">
         <v>1975</v>
       </c>
-      <c r="Y26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+      <c r="AB26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>25</v>
       </c>
@@ -6779,7 +6033,7 @@
       </c>
       <c r="M27" s="3">
         <f t="shared" si="2"/>
-        <v>0.6455903082800466</v>
+        <v>0.3544096917199534</v>
       </c>
       <c r="N27" s="3"/>
       <c r="O27" t="str">
@@ -6802,17 +6056,26 @@
       <c r="T27" t="s">
         <v>34</v>
       </c>
+      <c r="U27">
+        <v>874</v>
+      </c>
+      <c r="V27">
+        <v>2313</v>
+      </c>
       <c r="W27">
+        <v>30963.288358958253</v>
+      </c>
+      <c r="Z27">
         <v>1976</v>
       </c>
-      <c r="X27">
-        <v>1</v>
-      </c>
-      <c r="Y27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+      <c r="AA27">
+        <v>1</v>
+      </c>
+      <c r="AB27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>26</v>
       </c>
@@ -6851,17 +6114,26 @@
       <c r="T28" t="s">
         <v>37</v>
       </c>
+      <c r="U28">
+        <v>862</v>
+      </c>
+      <c r="V28">
+        <v>2340</v>
+      </c>
       <c r="W28">
+        <v>21296.064959400352</v>
+      </c>
+      <c r="Z28">
         <v>1977</v>
       </c>
-      <c r="X28">
-        <v>1</v>
-      </c>
-      <c r="Y28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+      <c r="AA28">
+        <v>1</v>
+      </c>
+      <c r="AB28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>27</v>
       </c>
@@ -6909,17 +6181,26 @@
       <c r="T29" t="s">
         <v>38</v>
       </c>
+      <c r="U29">
+        <v>1251</v>
+      </c>
+      <c r="V29">
+        <v>3431</v>
+      </c>
       <c r="W29">
+        <v>28533.746262281049</v>
+      </c>
+      <c r="Z29">
         <v>1978</v>
       </c>
-      <c r="X29">
-        <v>1</v>
-      </c>
-      <c r="Y29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+      <c r="AA29">
+        <v>1</v>
+      </c>
+      <c r="AB29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>28</v>
       </c>
@@ -6967,17 +6248,26 @@
       <c r="T30" t="s">
         <v>33</v>
       </c>
+      <c r="U30">
+        <v>1222</v>
+      </c>
+      <c r="V30">
+        <v>3602</v>
+      </c>
       <c r="W30">
+        <v>23680.555555555547</v>
+      </c>
+      <c r="Z30">
         <v>1979</v>
       </c>
-      <c r="X30">
+      <c r="AA30">
         <v>2</v>
       </c>
-      <c r="Y30">
+      <c r="AB30">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>29</v>
       </c>
@@ -7025,14 +6315,23 @@
       <c r="T31" t="s">
         <v>47</v>
       </c>
+      <c r="U31">
+        <v>1443</v>
+      </c>
+      <c r="V31">
+        <v>4477</v>
+      </c>
       <c r="W31">
+        <v>25807.432432432397</v>
+      </c>
+      <c r="Z31">
         <v>1980</v>
       </c>
-      <c r="X31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+      <c r="AA31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>30</v>
       </c>
@@ -7077,14 +6376,23 @@
       <c r="T32" t="s">
         <v>51</v>
       </c>
+      <c r="U32">
+        <v>1677</v>
+      </c>
+      <c r="V32">
+        <v>5494</v>
+      </c>
       <c r="W32">
+        <v>26790.545251708249</v>
+      </c>
+      <c r="Z32">
         <v>1982</v>
       </c>
-      <c r="Y32">
+      <c r="AB32">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>31</v>
       </c>
@@ -7132,14 +6440,23 @@
       <c r="T33" t="s">
         <v>57</v>
       </c>
+      <c r="U33">
+        <v>2415</v>
+      </c>
+      <c r="V33">
+        <v>6814</v>
+      </c>
       <c r="W33">
+        <v>27107.487268393099</v>
+      </c>
+      <c r="Z33">
         <v>1983</v>
       </c>
-      <c r="Y33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+      <c r="AB33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>32</v>
       </c>
@@ -7184,14 +6501,23 @@
       <c r="T34" t="s">
         <v>55</v>
       </c>
+      <c r="U34">
+        <v>1858</v>
+      </c>
+      <c r="V34">
+        <v>7409</v>
+      </c>
       <c r="W34">
+        <v>18636.020287039999</v>
+      </c>
+      <c r="Z34">
         <v>1984</v>
       </c>
-      <c r="Y34">
+      <c r="AB34">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F35" t="s">
         <v>44</v>
       </c>
@@ -7230,17 +6556,26 @@
       <c r="T35" t="s">
         <v>40</v>
       </c>
+      <c r="U35">
+        <v>1993</v>
+      </c>
+      <c r="V35">
+        <v>7443</v>
+      </c>
       <c r="W35">
+        <v>19815.0699448919</v>
+      </c>
+      <c r="Z35">
         <v>1985</v>
       </c>
-      <c r="X35">
-        <v>1</v>
-      </c>
-      <c r="Y35">
+      <c r="AA35">
+        <v>1</v>
+      </c>
+      <c r="AB35">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F36" t="s">
         <v>45</v>
       </c>
@@ -7279,17 +6614,26 @@
       <c r="T36" t="s">
         <v>61</v>
       </c>
+      <c r="U36">
+        <v>2173</v>
+      </c>
+      <c r="V36">
+        <v>8120</v>
+      </c>
       <c r="W36">
+        <v>17820.84912076165</v>
+      </c>
+      <c r="Z36">
         <v>1986</v>
       </c>
-      <c r="X36">
+      <c r="AA36">
         <v>4</v>
       </c>
-      <c r="Y36">
+      <c r="AB36">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F37" t="s">
         <v>46</v>
       </c>
@@ -7328,17 +6672,26 @@
       <c r="T37" t="s">
         <v>62</v>
       </c>
+      <c r="U37">
+        <v>2510</v>
+      </c>
+      <c r="V37">
+        <v>8176</v>
+      </c>
       <c r="W37">
+        <v>31437.394722066249</v>
+      </c>
+      <c r="Z37">
         <v>1987</v>
       </c>
-      <c r="X37">
+      <c r="AA37">
         <v>4</v>
       </c>
-      <c r="Y37">
+      <c r="AB37">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F38" t="s">
         <v>47</v>
       </c>
@@ -7377,17 +6730,26 @@
       <c r="T38" t="s">
         <v>78</v>
       </c>
+      <c r="U38">
+        <v>2541</v>
+      </c>
+      <c r="V38">
+        <v>8180</v>
+      </c>
       <c r="W38">
+        <v>19999.067251189252</v>
+      </c>
+      <c r="Z38">
         <v>1988</v>
       </c>
-      <c r="X38">
+      <c r="AA38">
         <v>4</v>
       </c>
-      <c r="Y38">
+      <c r="AB38">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F39" t="s">
         <v>48</v>
       </c>
@@ -7426,17 +6788,26 @@
       <c r="T39" t="s">
         <v>36</v>
       </c>
+      <c r="U39">
+        <v>2710</v>
+      </c>
+      <c r="V39">
+        <v>8476</v>
+      </c>
       <c r="W39">
+        <v>29669.229393885202</v>
+      </c>
+      <c r="Z39">
         <v>1989</v>
       </c>
-      <c r="X39">
+      <c r="AA39">
         <v>13</v>
       </c>
-      <c r="Y39">
+      <c r="AB39">
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F40" t="s">
         <v>49</v>
       </c>
@@ -7475,17 +6846,26 @@
       <c r="T40" t="s">
         <v>54</v>
       </c>
+      <c r="U40">
+        <v>2957</v>
+      </c>
+      <c r="V40">
+        <v>8854</v>
+      </c>
       <c r="W40">
+        <v>21679.790026246701</v>
+      </c>
+      <c r="Z40">
         <v>1990</v>
       </c>
-      <c r="X40">
+      <c r="AA40">
         <v>7</v>
       </c>
-      <c r="Y40">
+      <c r="AB40">
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F41" t="s">
         <v>50</v>
       </c>
@@ -7524,17 +6904,26 @@
       <c r="T41" t="s">
         <v>50</v>
       </c>
+      <c r="U41">
+        <v>3040</v>
+      </c>
+      <c r="V41">
+        <v>11106</v>
+      </c>
       <c r="W41">
+        <v>18684.43376219425</v>
+      </c>
+      <c r="Z41">
         <v>1991</v>
       </c>
-      <c r="X41">
+      <c r="AA41">
         <v>14</v>
       </c>
-      <c r="Y41">
+      <c r="AB41">
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F42" t="s">
         <v>51</v>
       </c>
@@ -7573,17 +6962,26 @@
       <c r="T42" t="s">
         <v>42</v>
       </c>
+      <c r="U42">
+        <v>3986</v>
+      </c>
+      <c r="V42">
+        <v>16607</v>
+      </c>
       <c r="W42">
+        <v>20784.004273296749</v>
+      </c>
+      <c r="Z42">
         <v>1992</v>
       </c>
-      <c r="X42">
+      <c r="AA42">
         <v>25</v>
       </c>
-      <c r="Y42">
+      <c r="AB42">
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F43" t="s">
         <v>52</v>
       </c>
@@ -7622,17 +7020,26 @@
       <c r="T43" t="s">
         <v>48</v>
       </c>
+      <c r="U43">
+        <v>6989</v>
+      </c>
+      <c r="V43">
+        <v>20605</v>
+      </c>
       <c r="W43">
+        <v>19287.345075016299</v>
+      </c>
+      <c r="Z43">
         <v>1993</v>
       </c>
-      <c r="X43">
+      <c r="AA43">
         <v>26</v>
       </c>
-      <c r="Y43">
+      <c r="AB43">
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F44" t="s">
         <v>53</v>
       </c>
@@ -7671,17 +7078,26 @@
       <c r="T44" t="s">
         <v>39</v>
       </c>
+      <c r="U44">
+        <v>7412</v>
+      </c>
+      <c r="V44">
+        <v>30902</v>
+      </c>
       <c r="W44">
+        <v>20535.443963042202</v>
+      </c>
+      <c r="Z44">
         <v>1994</v>
       </c>
-      <c r="X44">
+      <c r="AA44">
         <v>35</v>
       </c>
-      <c r="Y44">
+      <c r="AB44">
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F45" t="s">
         <v>54</v>
       </c>
@@ -7720,17 +7136,26 @@
       <c r="T45" t="s">
         <v>66</v>
       </c>
+      <c r="U45">
+        <v>7716</v>
+      </c>
+      <c r="V45">
+        <v>31632</v>
+      </c>
       <c r="W45">
+        <v>19790.459489681798</v>
+      </c>
+      <c r="Z45">
         <v>1995</v>
       </c>
-      <c r="X45">
+      <c r="AA45">
         <v>45</v>
       </c>
-      <c r="Y45">
+      <c r="AB45">
         <v>105</v>
       </c>
     </row>
-    <row r="46" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F46" t="s">
         <v>55</v>
       </c>
@@ -7769,17 +7194,26 @@
       <c r="T46" t="s">
         <v>45</v>
       </c>
+      <c r="U46">
+        <v>10517</v>
+      </c>
+      <c r="V46">
+        <v>30228</v>
+      </c>
       <c r="W46">
+        <v>21175.84979752115</v>
+      </c>
+      <c r="Z46">
         <v>1996</v>
       </c>
-      <c r="X46">
+      <c r="AA46">
         <v>66</v>
       </c>
-      <c r="Y46">
+      <c r="AB46">
         <v>107</v>
       </c>
     </row>
-    <row r="47" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F47" t="s">
         <v>56</v>
       </c>
@@ -7818,17 +7252,26 @@
       <c r="T47" t="s">
         <v>77</v>
       </c>
+      <c r="U47">
+        <v>10830</v>
+      </c>
+      <c r="V47">
+        <v>30129</v>
+      </c>
       <c r="W47">
+        <v>20610.732683903399</v>
+      </c>
+      <c r="Z47">
         <v>1997</v>
       </c>
-      <c r="X47">
+      <c r="AA47">
         <v>85</v>
       </c>
-      <c r="Y47">
+      <c r="AB47">
         <v>173</v>
       </c>
     </row>
-    <row r="48" spans="2:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F48" t="s">
         <v>57</v>
       </c>
@@ -7848,17 +7291,17 @@
         <v>3</v>
       </c>
       <c r="S48" s="5"/>
-      <c r="W48">
+      <c r="Z48">
         <v>1998</v>
       </c>
-      <c r="X48">
+      <c r="AA48">
         <v>121</v>
       </c>
-      <c r="Y48">
+      <c r="AB48">
         <v>232</v>
       </c>
     </row>
-    <row r="49" spans="6:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="49" spans="6:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F49" t="s">
         <v>58</v>
       </c>
@@ -7869,17 +7312,17 @@
         <v>1806</v>
       </c>
       <c r="S49" s="5"/>
-      <c r="W49">
+      <c r="Z49">
         <v>1999</v>
       </c>
-      <c r="X49">
+      <c r="AA49">
         <v>166</v>
       </c>
-      <c r="Y49">
+      <c r="AB49">
         <v>330</v>
       </c>
     </row>
-    <row r="50" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="50" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F50" t="s">
         <v>59</v>
       </c>
@@ -7913,17 +7356,17 @@
       <c r="T50" t="s">
         <v>17</v>
       </c>
-      <c r="W50">
+      <c r="Z50">
         <v>2000</v>
       </c>
-      <c r="X50">
+      <c r="AA50">
         <v>225</v>
       </c>
-      <c r="Y50">
+      <c r="AB50">
         <v>466</v>
       </c>
     </row>
-    <row r="51" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="51" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F51" t="s">
         <v>60</v>
       </c>
@@ -7957,17 +7400,17 @@
       <c r="T51">
         <v>1375</v>
       </c>
-      <c r="W51">
+      <c r="Z51">
         <v>2001</v>
       </c>
-      <c r="X51">
+      <c r="AA51">
         <v>252</v>
       </c>
-      <c r="Y51">
+      <c r="AB51">
         <v>456</v>
       </c>
     </row>
-    <row r="52" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="52" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F52" t="s">
         <v>61</v>
       </c>
@@ -8004,17 +7447,17 @@
       <c r="T52">
         <v>3338</v>
       </c>
-      <c r="W52">
+      <c r="Z52">
         <v>2002</v>
       </c>
-      <c r="X52">
+      <c r="AA52">
         <v>1382</v>
       </c>
-      <c r="Y52">
+      <c r="AB52">
         <v>1088</v>
       </c>
     </row>
-    <row r="53" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="53" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F53" t="s">
         <v>62</v>
       </c>
@@ -8051,17 +7494,17 @@
       <c r="T53">
         <v>33139</v>
       </c>
-      <c r="W53">
+      <c r="Z53">
         <v>2003</v>
       </c>
-      <c r="X53">
+      <c r="AA53">
         <v>3518</v>
       </c>
-      <c r="Y53">
+      <c r="AB53">
         <v>2130</v>
       </c>
     </row>
-    <row r="54" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="54" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F54" t="s">
         <v>63</v>
       </c>
@@ -8098,17 +7541,17 @@
       <c r="T54">
         <v>39374</v>
       </c>
-      <c r="W54">
+      <c r="Z54">
         <v>2004</v>
       </c>
-      <c r="X54">
+      <c r="AA54">
         <v>5637</v>
       </c>
-      <c r="Y54">
+      <c r="AB54">
         <v>3100</v>
       </c>
     </row>
-    <row r="55" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="55" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F55" t="s">
         <v>64</v>
       </c>
@@ -8145,17 +7588,17 @@
       <c r="T55">
         <v>32653</v>
       </c>
-      <c r="W55">
+      <c r="Z55">
         <v>2005</v>
       </c>
-      <c r="X55">
+      <c r="AA55">
         <v>8306</v>
       </c>
-      <c r="Y55">
+      <c r="AB55">
         <v>4453</v>
       </c>
     </row>
-    <row r="56" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="56" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F56" t="s">
         <v>65</v>
       </c>
@@ -8192,17 +7635,17 @@
       <c r="T56">
         <v>8828</v>
       </c>
-      <c r="W56">
+      <c r="Z56">
         <v>2006</v>
       </c>
-      <c r="X56">
+      <c r="AA56">
         <v>13387</v>
       </c>
-      <c r="Y56">
+      <c r="AB56">
         <v>7060</v>
       </c>
     </row>
-    <row r="57" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="57" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F57" t="s">
         <v>66</v>
       </c>
@@ -8239,17 +7682,17 @@
       <c r="T57">
         <v>3585</v>
       </c>
-      <c r="W57">
+      <c r="Z57">
         <v>2007</v>
       </c>
-      <c r="X57">
+      <c r="AA57">
         <v>19204</v>
       </c>
-      <c r="Y57">
+      <c r="AB57">
         <v>9837</v>
       </c>
     </row>
-    <row r="58" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="58" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F58" t="s">
         <v>67</v>
       </c>
@@ -8286,17 +7729,17 @@
       <c r="T58">
         <v>1262</v>
       </c>
-      <c r="W58">
+      <c r="Z58">
         <v>2008</v>
       </c>
-      <c r="X58">
+      <c r="AA58">
         <v>22247</v>
       </c>
-      <c r="Y58">
+      <c r="AB58">
         <v>11400</v>
       </c>
     </row>
-    <row r="59" spans="6:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="59" spans="6:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F59" t="s">
         <v>68</v>
       </c>
@@ -8325,17 +7768,17 @@
         <v>7958</v>
       </c>
       <c r="S59" s="5"/>
-      <c r="W59">
+      <c r="Z59">
         <v>2009</v>
       </c>
-      <c r="X59">
+      <c r="AA59">
         <v>19091</v>
       </c>
-      <c r="Y59">
+      <c r="AB59">
         <v>9768</v>
       </c>
     </row>
-    <row r="60" spans="6:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="60" spans="6:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F60" t="s">
         <v>69</v>
       </c>
@@ -8364,17 +7807,17 @@
         <v>7260</v>
       </c>
       <c r="S60" s="5"/>
-      <c r="W60">
+      <c r="Z60">
         <v>2010</v>
       </c>
-      <c r="X60">
+      <c r="AA60">
         <v>45687</v>
       </c>
-      <c r="Y60">
+      <c r="AB60">
         <v>22783</v>
       </c>
     </row>
-    <row r="61" spans="6:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="61" spans="6:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F61" t="s">
         <v>70</v>
       </c>
@@ -8394,17 +7837,17 @@
         <v>5891</v>
       </c>
       <c r="S61" s="5"/>
-      <c r="W61">
+      <c r="Z61">
         <v>2011</v>
       </c>
-      <c r="X61">
+      <c r="AA61">
         <v>40887</v>
       </c>
-      <c r="Y61">
+      <c r="AB61">
         <v>20406</v>
       </c>
     </row>
-    <row r="62" spans="6:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="62" spans="6:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F62" t="s">
         <v>71</v>
       </c>
@@ -8424,17 +7867,17 @@
         <v>5291</v>
       </c>
       <c r="S62" s="5"/>
-      <c r="W62">
+      <c r="Z62">
         <v>2012</v>
       </c>
-      <c r="X62">
+      <c r="AA62">
         <v>41639</v>
       </c>
-      <c r="Y62">
+      <c r="AB62">
         <v>21305</v>
       </c>
     </row>
-    <row r="63" spans="6:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="63" spans="6:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F63" t="s">
         <v>72</v>
       </c>
@@ -8454,17 +7897,17 @@
         <v>4503</v>
       </c>
       <c r="S63" s="5"/>
-      <c r="W63">
+      <c r="Z63">
         <v>2013</v>
       </c>
-      <c r="X63">
+      <c r="AA63">
         <v>15271</v>
       </c>
-      <c r="Y63">
+      <c r="AB63">
         <v>7758</v>
       </c>
     </row>
-    <row r="64" spans="6:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="64" spans="6:28" ht="15" x14ac:dyDescent="0.35">
       <c r="F64" t="s">
         <v>73</v>
       </c>
@@ -8484,13 +7927,13 @@
         <v>3835</v>
       </c>
       <c r="S64" s="5"/>
-      <c r="W64">
+      <c r="Z64">
         <v>2014</v>
       </c>
-      <c r="X64">
+      <c r="AA64">
         <v>642</v>
       </c>
-      <c r="Y64">
+      <c r="AB64">
         <v>315</v>
       </c>
     </row>
@@ -12588,874 +12031,874 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="12" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="13" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="10" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="11">
         <v>0.38888888888888801</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>0.36783042394014898</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>0.32210834553440698</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="9">
         <v>0.36288998357963798</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="9">
         <v>0.32258064516128998</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="9">
         <v>0.33333333333333298</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="9">
         <v>0.35616438356164298</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="9">
         <v>0.27272727272727199</v>
       </c>
-      <c r="K3" s="14">
+      <c r="K3" s="11">
         <v>0.5</v>
       </c>
-      <c r="L3" s="14">
+      <c r="L3" s="11">
         <v>0.44444444444444398</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>0.367049808429118</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>0.33281855715591402</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>0.330718734219828</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="9">
         <v>0.34280422300426</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="9">
         <v>0.34169034486600902</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="9">
         <v>0.32338425381903602</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="9">
         <v>0.32095096582466498</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="9">
         <v>0.31640625</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="11">
         <v>0.41509433962264097</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L4" s="11">
         <v>0.45961002785515298</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>0.359837854692859</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>0.33837948252383099</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>0.34103177459302603</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>0.347936808419534</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="9">
         <v>0.34228814438336203</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="9">
         <v>0.33770585299778999</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="9">
         <v>0.31908704408145</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="9">
         <v>0.33600641539695197</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="9">
         <v>0.29670329670329598</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="11">
         <v>0.43768996960486301</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="11">
         <v>0.38073394495412799</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>0.35706554419723302</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>0.355103578154425</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <v>0.35471863367637302</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="9">
         <v>0.35162950257289799</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="9">
         <v>0.34274531730500402</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="9">
         <v>0.34994913530010102</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="9">
         <v>0.33495145631067902</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="9">
         <v>0.22222222222222199</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="11">
         <v>0.45652173913043398</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="12" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
     </row>
     <row r="9" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="13" t="s">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="K9" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="L9" s="10" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="13">
         <v>0.55681818181818099</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="13">
         <v>0.68226120857699801</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="13">
         <v>0.70350404312668402</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="13">
         <v>0.65909090909090895</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="13">
         <v>0.59799999999999998</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="13">
         <v>0.581395348837209</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10" s="13">
         <v>0.52</v>
       </c>
-      <c r="J10" s="17">
+      <c r="J10" s="14">
         <v>0.83333333333333304</v>
       </c>
-      <c r="K10" s="16">
+      <c r="K10" s="13">
         <v>0.57142857142857095</v>
       </c>
-      <c r="L10" s="17">
+      <c r="L10" s="14">
         <v>0.8</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="13" t="s">
+      <c r="A11" s="17"/>
+      <c r="B11" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="13">
         <v>0.36104513064132998</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="13">
         <v>0.36498229803669102</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="13">
         <v>0.40630712979890299</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="13">
         <v>0.39017808958445699</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="13">
         <v>0.36206896551724099</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="13">
         <v>0.34735202492211797</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="13">
         <v>0.27835051546391698</v>
       </c>
-      <c r="J11" s="16">
+      <c r="J11" s="13">
         <v>0.31578947368421001</v>
       </c>
-      <c r="K11" s="16">
+      <c r="K11" s="13">
         <v>0.15384615384615299</v>
       </c>
-      <c r="L11" s="17">
+      <c r="L11" s="14">
         <v>0.70270270270270196</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="13" t="s">
+      <c r="A12" s="17"/>
+      <c r="B12" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="13">
         <v>0.34461438333875599</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="13">
         <v>0.32666709126807197</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="13">
         <v>0.329936305732484</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="13">
         <v>0.34636205612118198</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12" s="13">
         <v>0.336808051761322</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="13">
         <v>0.329483282674772</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I12" s="13">
         <v>0.30674586338565901</v>
       </c>
-      <c r="J12" s="16">
+      <c r="J12" s="13">
         <v>0.33250620347394499</v>
       </c>
-      <c r="K12" s="16">
+      <c r="K12" s="13">
         <v>0.46938775510204001</v>
       </c>
-      <c r="L12" s="16">
+      <c r="L12" s="13">
         <v>0.375</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="13" t="s">
+      <c r="A13" s="17"/>
+      <c r="B13" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="13">
         <v>0.36906077348066202</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="13">
         <v>0.33072413914142301</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="13">
         <v>0.32932522755516702</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="13">
         <v>0.34289543264877298</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13" s="13">
         <v>0.33560664393355999</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="13">
         <v>0.3296011196641</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13" s="13">
         <v>0.33073206986250397</v>
       </c>
-      <c r="J13" s="16">
+      <c r="J13" s="13">
         <v>0.34168865435356199</v>
       </c>
-      <c r="K13" s="16">
+      <c r="K13" s="13">
         <v>0.217391304347826</v>
       </c>
-      <c r="L13" s="16">
+      <c r="L13" s="13">
         <v>0.42587601078167098</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="13" t="s">
+      <c r="A14" s="17"/>
+      <c r="B14" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="13">
         <v>0.37425742574257398</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="13">
         <v>0.33287460535902202</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="13">
         <v>0.33521876559640601</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="13">
         <v>0.33934388087482498</v>
       </c>
-      <c r="G14" s="16">
+      <c r="G14" s="13">
         <v>0.34313279330117402</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="13">
         <v>0.33103843947217398</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="13">
         <v>0.33355525965379401</v>
       </c>
-      <c r="J14" s="16">
+      <c r="J14" s="13">
         <v>0.28527607361963098</v>
       </c>
-      <c r="K14" s="16">
+      <c r="K14" s="13">
         <v>0.31818181818181801</v>
       </c>
-      <c r="L14" s="16">
+      <c r="L14" s="13">
         <v>0.44015444015444</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
-      <c r="B15" s="13" t="s">
+      <c r="A15" s="17"/>
+      <c r="B15" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="13">
         <v>0.41450777202072497</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="13">
         <v>0.336713138994507</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="13">
         <v>0.33691395322815199</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="13">
         <v>0.34367853642600399</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="13">
         <v>0.34658785599140202</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="13">
         <v>0.33854166666666602</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="13">
         <v>0.328125</v>
       </c>
-      <c r="J15" s="16">
+      <c r="J15" s="13">
         <v>0.31410256410256399</v>
       </c>
-      <c r="K15" s="16">
+      <c r="K15" s="13">
         <v>0.375</v>
       </c>
-      <c r="L15" s="16">
+      <c r="L15" s="13">
         <v>0.455696202531645</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
-      <c r="B16" s="13" t="s">
+      <c r="A16" s="17"/>
+      <c r="B16" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="13">
         <v>0.435294117647058</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="13">
         <v>0.34253246753246702</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="13">
         <v>0.33057471264367799</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="13">
         <v>0.341220698805838</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G16" s="13">
         <v>0.34807472359893199</v>
       </c>
-      <c r="H16" s="16">
+      <c r="H16" s="13">
         <v>0.32927756653992302</v>
       </c>
-      <c r="I16" s="16">
+      <c r="I16" s="13">
         <v>0.35127478753541003</v>
       </c>
-      <c r="J16" s="16">
+      <c r="J16" s="13">
         <v>0.32758620689655099</v>
       </c>
-      <c r="K16" s="16">
+      <c r="K16" s="13">
         <v>0.25</v>
       </c>
-      <c r="L16" s="16">
+      <c r="L16" s="13">
         <v>0.50892857142857095</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="13" t="s">
+      <c r="A17" s="17"/>
+      <c r="B17" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="13">
         <v>0.44827586206896503</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="13">
         <v>0.34788189987162998</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="13">
         <v>0.35380835380835302</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="13">
         <v>0.34663120567375799</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G17" s="13">
         <v>0.34398782343987799</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H17" s="13">
         <v>0.331738437001594</v>
       </c>
-      <c r="I17" s="16">
+      <c r="I17" s="13">
         <v>0.29936305732483998</v>
       </c>
-      <c r="J17" s="16">
+      <c r="J17" s="13">
         <v>0.25</v>
       </c>
-      <c r="K17" s="16">
+      <c r="K17" s="13">
         <v>0</v>
       </c>
-      <c r="L17" s="16">
+      <c r="L17" s="13">
         <v>0.31578947368421001</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="13" t="s">
+      <c r="A18" s="17"/>
+      <c r="B18" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="13">
         <v>0.45</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="13">
         <v>0.38095238095237999</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="13">
         <v>0.37041564792176002</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="13">
         <v>0.35122410546139299</v>
       </c>
-      <c r="G18" s="16">
+      <c r="G18" s="13">
         <v>0.38461538461538403</v>
       </c>
-      <c r="H18" s="16">
+      <c r="H18" s="13">
         <v>0.35199999999999998</v>
       </c>
-      <c r="I18" s="16">
+      <c r="I18" s="13">
         <v>0.4</v>
       </c>
-      <c r="J18" s="16">
+      <c r="J18" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="K18" s="16">
+      <c r="K18" s="13">
         <v>0</v>
       </c>
-      <c r="L18" s="16">
+      <c r="L18" s="13">
         <v>0.54545454545454497</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="13" t="s">
+      <c r="A19" s="17"/>
+      <c r="B19" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="13">
         <v>0.26315789473684198</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="13">
         <v>0.34146341463414598</v>
       </c>
-      <c r="E19" s="16">
+      <c r="E19" s="13">
         <v>0.40570175438596401</v>
       </c>
-      <c r="F19" s="16">
+      <c r="F19" s="13">
         <v>0.375494071146245</v>
       </c>
-      <c r="G19" s="16">
+      <c r="G19" s="13">
         <v>0.34732824427480902</v>
       </c>
-      <c r="H19" s="16">
+      <c r="H19" s="13">
         <v>0.369747899159663</v>
       </c>
-      <c r="I19" s="16">
+      <c r="I19" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="J19" s="16">
+      <c r="J19" s="13">
         <v>0.25</v>
       </c>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16">
+      <c r="K19" s="13"/>
+      <c r="L19" s="13">
         <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
-      <c r="B20" s="13" t="s">
+      <c r="A20" s="17"/>
+      <c r="B20" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20" s="13">
         <v>0.14285714285714199</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="13">
         <v>0.38983050847457601</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="13">
         <v>0.38725490196078399</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F20" s="13">
         <v>0.34146341463414598</v>
       </c>
-      <c r="G20" s="16">
+      <c r="G20" s="13">
         <v>0.41489361702127597</v>
       </c>
-      <c r="H20" s="16">
+      <c r="H20" s="13">
         <v>0.37254901960784298</v>
       </c>
-      <c r="I20" s="16">
+      <c r="I20" s="13">
         <v>0.214285714285714</v>
       </c>
-      <c r="J20" s="16">
+      <c r="J20" s="13">
         <v>0</v>
       </c>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16">
+      <c r="K20" s="13"/>
+      <c r="L20" s="13">
         <v>0.2</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="11"/>
-      <c r="B21" s="13" t="s">
+      <c r="A21" s="17"/>
+      <c r="B21" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="13">
         <v>0.57499999999999996</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="13">
         <v>0.37962962962962898</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F21" s="13">
         <v>0.34166666666666601</v>
       </c>
-      <c r="G21" s="16">
+      <c r="G21" s="13">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H21" s="16">
+      <c r="H21" s="13">
         <v>0.47058823529411697</v>
       </c>
-      <c r="I21" s="16">
+      <c r="I21" s="13">
         <v>0.22222222222222199</v>
       </c>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16">
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13">
         <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
-      <c r="B22" s="13" t="s">
+      <c r="A22" s="17"/>
+      <c r="B22" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C22" s="16">
+      <c r="C22" s="13">
         <v>0.5</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="13">
         <v>0.56666666666666599</v>
       </c>
-      <c r="E22" s="16">
+      <c r="E22" s="13">
         <v>0.5</v>
       </c>
-      <c r="F22" s="16">
+      <c r="F22" s="13">
         <v>0.36065573770491799</v>
       </c>
-      <c r="G22" s="16">
+      <c r="G22" s="13">
         <v>0.46875</v>
       </c>
-      <c r="H22" s="16">
+      <c r="H22" s="13">
         <v>0.52631578947368396</v>
       </c>
-      <c r="I22" s="16">
+      <c r="I22" s="13">
         <v>0.42857142857142799</v>
       </c>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="17">
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
-      <c r="B23" s="13" t="s">
+      <c r="A23" s="17"/>
+      <c r="B23" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16">
+      <c r="C23" s="13"/>
+      <c r="D23" s="13">
         <v>0.46153846153846101</v>
       </c>
-      <c r="E23" s="16">
+      <c r="E23" s="13">
         <v>0.40540540540540498</v>
       </c>
-      <c r="F23" s="16">
+      <c r="F23" s="13">
         <v>0.4</v>
       </c>
-      <c r="G23" s="16">
+      <c r="G23" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="H23" s="16">
+      <c r="H23" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="I23" s="17">
-        <v>1</v>
-      </c>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16">
+      <c r="I23" s="14">
+        <v>1</v>
+      </c>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
-      <c r="B24" s="13" t="s">
+      <c r="A24" s="17"/>
+      <c r="B24" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="16">
+      <c r="C24" s="15"/>
+      <c r="D24" s="13">
         <v>0.42857142857142799</v>
       </c>
-      <c r="E24" s="16">
+      <c r="E24" s="13">
         <v>0.5625</v>
       </c>
-      <c r="F24" s="16">
+      <c r="F24" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="G24" s="16">
+      <c r="G24" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="H24" s="16">
+      <c r="H24" s="13">
         <v>0.25</v>
       </c>
-      <c r="I24" s="16">
+      <c r="I24" s="13">
         <v>0</v>
       </c>
-      <c r="J24" s="17">
-        <v>1</v>
-      </c>
-      <c r="K24" s="18"/>
-      <c r="L24" s="16">
+      <c r="J24" s="14">
+        <v>1</v>
+      </c>
+      <c r="K24" s="15"/>
+      <c r="L24" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
-      <c r="B25" s="13" t="s">
+      <c r="A25" s="17"/>
+      <c r="B25" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="16">
+      <c r="C25" s="15"/>
+      <c r="D25" s="13">
         <v>0.5</v>
       </c>
-      <c r="E25" s="16">
+      <c r="E25" s="13">
         <v>0.5</v>
       </c>
-      <c r="F25" s="16">
+      <c r="F25" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="G25" s="17">
+      <c r="G25" s="14">
         <v>0.8</v>
       </c>
-      <c r="H25" s="16">
+      <c r="H25" s="13">
         <v>0.6</v>
       </c>
-      <c r="I25" s="16">
+      <c r="I25" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="16">
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="11"/>
-      <c r="B26" s="13" t="s">
+      <c r="A26" s="17"/>
+      <c r="B26" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="17">
-        <v>1</v>
-      </c>
-      <c r="E26" s="16">
+      <c r="C26" s="15"/>
+      <c r="D26" s="14">
+        <v>1</v>
+      </c>
+      <c r="E26" s="13">
         <v>0</v>
       </c>
-      <c r="F26" s="16">
+      <c r="F26" s="13">
         <v>0.28571428571428498</v>
       </c>
-      <c r="G26" s="17">
+      <c r="G26" s="14">
         <v>0.66666666666666596</v>
       </c>
-      <c r="H26" s="16">
+      <c r="H26" s="13">
         <v>0.5</v>
       </c>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
     </row>
     <row r="27" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="11"/>
-      <c r="B27" s="13" t="s">
+      <c r="A27" s="17"/>
+      <c r="B27" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="16">
+      <c r="C27" s="15"/>
+      <c r="D27" s="13">
         <v>0</v>
       </c>
-      <c r="E27" s="16">
+      <c r="E27" s="13">
         <v>0.25</v>
       </c>
-      <c r="F27" s="16">
+      <c r="F27" s="13">
         <v>0.16666666666666599</v>
       </c>
-      <c r="G27" s="16">
+      <c r="G27" s="13">
         <v>0.5</v>
       </c>
-      <c r="H27" s="18"/>
-      <c r="I27" s="16">
+      <c r="H27" s="15"/>
+      <c r="I27" s="13">
         <v>0.5</v>
       </c>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
     </row>
     <row r="28" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="11"/>
-      <c r="B28" s="13" t="s">
+      <c r="A28" s="17"/>
+      <c r="B28" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="17">
-        <v>1</v>
-      </c>
-      <c r="F28" s="16">
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="14">
+        <v>1</v>
+      </c>
+      <c r="F28" s="13">
         <v>0</v>
       </c>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="17">
-        <v>1</v>
-      </c>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="14">
+        <v>1</v>
+      </c>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -13528,7 +12971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2808B69F-E6D1-480C-BA78-6E297A9A26C0}">
   <dimension ref="B2:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -13538,10 +12981,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="18"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -13555,7 +12998,7 @@
       <c r="B4" t="s">
         <v>144</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="12">
         <v>11869.8570989203</v>
       </c>
     </row>
@@ -13563,7 +13006,7 @@
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="12">
         <v>1093.4368310766699</v>
       </c>
     </row>
@@ -13571,7 +13014,7 @@
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="12">
         <v>698.34771364557605</v>
       </c>
     </row>
@@ -13579,7 +13022,7 @@
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="12">
         <v>365.45830508648402</v>
       </c>
     </row>
@@ -13587,7 +13030,7 @@
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="12">
         <v>349.23024765668498</v>
       </c>
     </row>
@@ -13595,7 +13038,7 @@
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="12">
         <v>133.00166341609301</v>
       </c>
     </row>
@@ -13603,7 +13046,7 @@
       <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="12">
         <v>93.305188392097094</v>
       </c>
     </row>
@@ -13611,7 +13054,7 @@
       <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="12">
         <v>82.105560753168803</v>
       </c>
     </row>
@@ -13619,7 +13062,7 @@
       <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="12">
         <v>59.257995713963297</v>
       </c>
     </row>
@@ -13627,7 +13070,7 @@
       <c r="B13" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="12">
         <v>23.737361633894398</v>
       </c>
     </row>
@@ -13635,7 +13078,7 @@
       <c r="B14" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="12">
         <v>23.371714450063401</v>
       </c>
     </row>
@@ -13643,7 +13086,7 @@
       <c r="B15" t="s">
         <v>138</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="12">
         <v>7.3364809482583802</v>
       </c>
     </row>
@@ -13651,7 +13094,7 @@
       <c r="B16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="12">
         <v>2.0510437406890598</v>
       </c>
     </row>
@@ -13659,7 +13102,7 @@
       <c r="B17" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="12">
         <v>0.73113998038038097</v>
       </c>
     </row>
@@ -13667,7 +13110,7 @@
       <c r="B18" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="12">
         <v>0.21377281914893501</v>
       </c>
     </row>

</xml_diff>

<commit_message>
stuff that will never be pushed
</commit_message>
<xml_diff>
--- a/regressor and classifier importances.xlsx
+++ b/regressor and classifier importances.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a38cc7a04266740c/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minna\OneDrive\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="435" documentId="8_{E93A6E45-9447-44B2-A386-D641E629DBB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EE6DDEE8-17E3-438D-B0AD-9C9C87EFEE5C}"/>
+  <xr:revisionPtr revIDLastSave="438" documentId="8_{E93A6E45-9447-44B2-A386-D641E629DBB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{801BDEAC-4EDE-4F90-A476-768862A8DE41}"/>
   <bookViews>
-    <workbookView xWindow="3552" yWindow="1200" windowWidth="13668" windowHeight="4500" firstSheet="1" activeTab="1" xr2:uid="{789FB943-771A-4B19-9A66-979F3CA78A6C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{789FB943-771A-4B19-9A66-979F3CA78A6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Original Importances" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,6 @@
     <sheet name="Heatmaps" sheetId="3" r:id="rId3"/>
     <sheet name="chi - 2" sheetId="4" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -4240,19 +4237,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4877,8 +4861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58B855E-757F-44CC-B7FE-FF60EBDD6187}">
   <dimension ref="B1:AC474"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4924,8 +4908,8 @@
         <v>62477</v>
       </c>
       <c r="J2" s="3">
-        <f>I3/SUM(H3:I3)</f>
-        <v>0.36385895304988114</v>
+        <f>I2/SUM(H2:I2)</f>
+        <v>0.32255016856223895</v>
       </c>
       <c r="P2" t="s">
         <v>86</v>
@@ -4970,8 +4954,8 @@
         <v>61077</v>
       </c>
       <c r="J3" s="3">
-        <f>I2/SUM(H2:I2)</f>
-        <v>0.32255016856223895</v>
+        <f>I3/SUM(H3:I3)</f>
+        <v>0.36385895304988114</v>
       </c>
       <c r="M3" t="s">
         <v>89</v>

</xml_diff>